<commit_message>
update version of survey with updated data
</commit_message>
<xml_diff>
--- a/Back_Questionnaire.xlsx
+++ b/Back_Questionnaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanpro/Dropbox/Equal/github/typeform/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanpro/Dropbox/Equal/git-perdev-dev/equal-survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1760BF-7073-B64F-B2BD-78ED510DCAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB6F080-3969-A74C-89A4-6CAA75E6D598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8680" yWindow="1420" windowWidth="40180" windowHeight="25100" xr2:uid="{C96B8C69-CC42-2D4D-A209-28F3A5CB5315}"/>
+    <workbookView xWindow="37300" yWindow="3020" windowWidth="29460" windowHeight="23340" xr2:uid="{C96B8C69-CC42-2D4D-A209-28F3A5CB5315}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="207">
   <si>
     <t>ID</t>
   </si>
@@ -62,10 +62,6 @@
     <t>Multichoice - Single</t>
   </si>
   <si>
-    <t>yes: 네.
-no: 아니요.</t>
-  </si>
-  <si>
     <t>common</t>
   </si>
   <si>
@@ -75,14 +71,6 @@
     <t>Multichoice - Single - Vertical</t>
   </si>
   <si>
-    <t>yes: 네.
-conditional: 항체가 검사를 통해 필요한 추가 접종만 진행하고 있어요.
-no: 아니요. 추가 접종을 하고 있지 않아요.</t>
-  </si>
-  <si>
-    <t>현재 임신 중인가요?</t>
-  </si>
-  <si>
     <t>최근 6개월 이내에 출산한 적이 있나요?</t>
   </si>
   <si>
@@ -92,205 +80,40 @@
     <t>최근 {@petname}의 체중에 변화가 있었나요?</t>
   </si>
   <si>
-    <t>decreased_significantly: 눈에 띄게 줄었어요.
-decreased_slightly: 조금 줄었어요.
-no_change: 아니요, 비슷해요.
-increased_slightly: 조금 늘었어요.
-increased_significantly: 눈에 띄게 늘었어요.</t>
-  </si>
-  <si>
-    <t>현재 고양이 헤르페스바이러스 감염 증상(재채기, 콧물, 결막염 등)이 있나요?</t>
-  </si>
-  <si>
-    <t>positive: 네.
-negative: 아니요.
-carrier: 아니요. 하지만 보균자에요.</t>
-  </si>
-  <si>
-    <t>animal_protein: 동물성 단백질 일반 사료 (곤충 단백질 포함)
-plant_protein: 식물성 단백질 일반 사료 (두부, 콩 단백질 등 포함)
-prescription_diet: 수의사 처방사료 (Royal Canin, Hill's, Purina, Velixer 등에서 생산한 처방식)
-cooked_meat: 화식류 제품 (기성제품, 집에서 직접 굽거나 조리한 고기 등 포함)
-raw_diet: 생식 및 동결건조 사료 (조리되지 않은 어류, 육류, 생고기 등 포함)</t>
-  </si>
-  <si>
-    <t>recommended_or_less: 권장량을 지켜서 주거나 적게 줘요.
-more_than_recommended: 권장량보다 많이 줘요.</t>
-  </si>
-  <si>
     <t>사료나 간식을 먹는 속도는 어떤가요?</t>
   </si>
   <si>
-    <t>fast: 주자마자 허겁지겁 순식간에 먹어요. 잘 씹지 않고 삼키는 것 같아요.
-moderate: 적당한 속도로 잘 씹어서 먹어요.
-slow: 아주 느리게 먹거나, 먹을 것에 별로 관심이 없어요.</t>
-  </si>
-  <si>
-    <t>최근 구토 또는 역류 증상을 나타낸 적이 있나요?</t>
-  </si>
-  <si>
-    <t>absent: 아니요.
-intermittent: 네, 이전부터 종종 있었어요.
-increased_recently: 네, 최근 들어서 심해졌어요.</t>
-  </si>
-  <si>
     <t>최근 대변의 상태는 어떤가요?</t>
   </si>
   <si>
-    <t>dry_hard: 건조하고 딱딱해요.
-dry_soft: 건조한 편이지만, 적당히 말랑해요.
-moist_soft: 습기가 있으면서 적당히 말랑해요. 가끔 주변에 살짝 묻어날 때도 있어요.
-loose: 무른 변을 보고 있어요. 거의 항상 주변에 많이 묻어나요.
-diarrhea : 설사 증상이 나타났어요.</t>
-  </si>
-  <si>
-    <t>최근 {@petname}에게 변비 증상이 있나요?</t>
-  </si>
-  <si>
-    <t>no: 아니요, 없어요.
-recent: 네, 최근에 변비가 생겼어요.
-chronic: 네, 예전부터 계속 변비가 있었어요.</t>
-  </si>
-  <si>
-    <t>최근 음수량에 변화가 있나요?</t>
-  </si>
-  <si>
-    <t>decreased: 줄었어요.
-stable: 비슷해요.
-increase: 늘었어요.</t>
-  </si>
-  <si>
     <t>최근 소변량에 변화가 있었나요?</t>
   </si>
   <si>
-    <t>decreased: 줄었어요.
-stable: 비슷해요.
-increased: 늘었어요.</t>
-  </si>
-  <si>
-    <t>최근 하루 소변 횟수에 변화가 있었나요?</t>
-  </si>
-  <si>
     <t>최근 소변 냄새가 심해졌나요?</t>
   </si>
   <si>
-    <t>normal: 아니요.
-strong: 네.</t>
-  </si>
-  <si>
-    <t>최근 {@petname}의 화장실 방문 빈도에 변화가 있나요?</t>
-  </si>
-  <si>
     <t>전신 목욕은 얼마나 자주 하나요?</t>
   </si>
   <si>
-    <t>no_bathing: 목욕을 시키고 있지 않아요.
-less_than_monthly: 1달에 1번 이하
-biweekly: 2주일에 1번
-weekly: 1주일에 1번
-twice_weekly: 1주일에 2번
-more_than_twice_weekly: 1주일에 3번 이상</t>
-  </si>
-  <si>
     <t>미용을 주기적으로 하나요?</t>
   </si>
   <si>
-    <t>regular: 네.
-not_regular: 아니요.</t>
-  </si>
-  <si>
     <t>미용은 주로 어디서 하나요?</t>
   </si>
   <si>
-    <t>home: 집에서 해요.
-shop_or_vet: 샵 또는 동물병원에서 해요.</t>
-  </si>
-  <si>
     <t>미용을 위해 마취를 하나요?</t>
   </si>
   <si>
-    <t>최근 6개월 내에 감염성 피부염(ex. 곰팡이, 세균 등)이 2번 이상 나타났나요?</t>
-  </si>
-  <si>
-    <t>주로 생활하는 실내 환경이 건조하지는 않나요?</t>
-  </si>
-  <si>
-    <t>dry_with_humidifier: 건조한 편이라 평소 가습기를 틀어놔요.
-dry_without_care: 건조한 편이지만 특별히 신경 쓰고 있지 않아요.
-not_dry: 건조하지 않아서 특별히 신경 쓰고 있지 않아요.
-humid: 건조하지 않고 오히려 습한 환경이에요.</t>
-  </si>
-  <si>
-    <t>최근 눈을 반복적으로 비비는 행동을 보인 적이 있나요?</t>
-  </si>
-  <si>
-    <t>never: 아니요, 그렇지 않아요.
-1-2_times_weekly: 일주일에 1-2회 정도 보여요.
-3-5_times_weekly: 일주일에 3-5회 정도 보여요.
-daily: 거의 매일 보여요.</t>
-  </si>
-  <si>
-    <t>혹시 입안에 염증이 있거나 나쁜 냄새가 난다면 최근에 심해졌나요?</t>
-  </si>
-  <si>
-    <t>absent: 아니요, 구취나 염증은 없어요.
-present: 염증은 있지만, 구취가 심해지진 않았어요.
-worsened: 네, 둘 다 심해졌어요.
-unconfirmed: 입안을 안 보여줘서 확인하기 어려워요.</t>
-  </si>
-  <si>
-    <t>가장 최근에 받은 스케일링은 언제인가요?</t>
-  </si>
-  <si>
-    <t>last_6_months: 6개월 내
-6_months_to_1_year: 6개월 초과, 1년 이내
-over_1_year_or_never: 1년 초과, 혹은 받은 적 없어요.</t>
-  </si>
-  <si>
-    <t>칫솔질을 하고 있나요?</t>
-  </si>
-  <si>
-    <t>everyday: 매일 해요.
-3_times_weekly: 일주일에 3회 이상 해요.
-only_toothpaste: 치약만 잇몸이나 치아에 발라주고 있거나, 마시는 물에 치석 방지 제품을 섞어줘요.
-never: 잘 못해주고 있어요.</t>
-  </si>
-  <si>
     <t>최근에 입을 벌리고 호흡하는 경우가 있었나요?</t>
   </si>
   <si>
     <t>최근 잠을 자거나 휴식을 취할 때, 코골이나 헉헉거림 등의 비정상적인 숨소리를 내나요?</t>
   </si>
   <si>
-    <t>never: 아니요, 안 그래요.
-1-2_times_weekly: 일주일에 1-2회 정도 비정상적인 숨소리를 내요.
-3-5_times_weekly: 일주일에 3-5회 정도 비정상적인 숨소리를 내요.
-daily: 매일 비정상적인 숨소리를 내요.</t>
-  </si>
-  <si>
-    <t>최근 캑캑거리는 증상이 자주 나타나나요?</t>
-  </si>
-  <si>
-    <t>none: 아니요, 안 그래요.
-occasional: 격한 운동 후 혹은 과하게 흥분하는 일이 있을 때만 캑캑거려요.
-frequent: 특별한 일이 없는데도 캑캑거리는 모습이 하루에 한두 번 정도 보여요.
-very_frequent: 특별한 일이 없는데도 캑캑거리는 모습이 하루에 네다섯 번 이상 보여요.</t>
-  </si>
-  <si>
     <t>{@petname}의 성격은 어떤가요?</t>
   </si>
   <si>
-    <t>excitable: 항상 격하게 흥분해요.
-calm_excitable: 때로는 격하지만, 평소에는 차분한 편이에요.
-peaceful_expressive: 꼬리를 살랑이거나 만져달라고 오는 등 평온한 방식으로 기분과 상태를 표현해요.
-Indifferent: 주변 환경 변화에 예민한 편은 아니에요. 성격이 무던해요.
-anxious_sensitive: 겁이 많고, 반려인과 멀어지거나 환경이 변화하면 많이 불안해하고 예민한 편이에요.</t>
-  </si>
-  <si>
     <t>dog</t>
-  </si>
-  <si>
-    <t>최근 급격한 성격의 변화가 있었나요?</t>
   </si>
   <si>
     <t>none: 아니요, 없었어요.
@@ -300,24 +123,6 @@
 specific_aggression: 네, 특정 부위를 만지려고 하면 짖거나 물려고 해요.</t>
   </si>
   <si>
-    <t>반려인이 잠깐 집을 비울 때, 어떻게 행동하나요?</t>
-  </si>
-  <si>
-    <t>immediate_barking: 나가자마자 짖기 시작해요.
-occasional_barking: 바로 짖지는 않지만, 종종 짖어요.
-indifferent: 별로 신경쓰지 않아요.</t>
-  </si>
-  <si>
-    <t>산책은 얼마나 오래 하나요?</t>
-  </si>
-  <si>
-    <t>none: 거의 활동량이 없어요.
-short: 10-30분 이내
-medium: 30-60분 이내
-long: 1시간 이상
-indoor: 산책을 자주 가진 않지만, 집안에서 활동량이 많아요.</t>
-  </si>
-  <si>
     <t>산책할 때 {@petname}의 상태는 어떤가요?</t>
   </si>
   <si>
@@ -328,69 +133,7 @@
 low_after_long_walk: 1시간 정도 걸으면 힘들어해요.</t>
   </si>
   <si>
-    <t>산책할 때 다리를 아파하는 증상이 있나요?</t>
-  </si>
-  <si>
-    <t>no_symptoms: 아니요, 그렇지 않아요.
-unstable_after_short_walk: 조금만 걸어도 다리를 떨거나, 절뚝이는 등 불안정해요.
-unstable_after_long_walk: 오래 걸으면 다리를 떨거나, 절뚝이는 등 불안정해요.</t>
-  </si>
-  <si>
-    <t>주로 생활하는 실내 공간은 어떤 바닥인가요?</t>
-  </si>
-  <si>
-    <t>slippery: 미끄러운 바닥 (예: 대리석)
-less_slippery: 조금 덜 미끄러운 바닥 (예: 나무 바닥)
-non_slippery: 미끄러짐이 거의 없는 바닥 (예: 장판)</t>
-  </si>
-  <si>
-    <t>미끄럼 방지 관련 제품을 사용하시나요?</t>
-  </si>
-  <si>
-    <t>pad_used: 미끄럼 방지 패드를 깔아놨어요.
-cream_used: 미끄럼 방지 크림을 바르고 있어요.
-both_used: 둘 다 사용하고 있어요.
-none_used: 둘 다 사용하지 않아요.</t>
-  </si>
-  <si>
-    <t>주로 생활하는 실내 공간의 가구 높이는 어떤가요?</t>
-  </si>
-  <si>
-    <t>low: 소파, 침대와 같은 가구가 없는 좌식 생활을 하거나, 저상형이에요.
-high: 소파, 침대 등 모두 높은 편이에요.
-high_stepped: 소파, 침대 등 모두 높지만, 계단식 구조로 되어있어요.</t>
-  </si>
-  <si>
-    <t>소파나 침대 등 높은 곳에 올라가고 내려갈 때, 어떻게 행동하나요?</t>
-  </si>
-  <si>
-    <t>runs_and_jumps: 달려와서 점프해요.
-requests_assistance: 반려인에게 올려 달라고 애원해요.
-uses_stairs_or_objects: 계단이나 주변 사물이나 이용해서 계단식으로 올라와요.
-avoids_climbing: 올라오지 않으려 해요.</t>
-  </si>
-  <si>
-    <t>두 발로 서려고 할 때, 반려인님은 어떻게 행동하시나요?</t>
-  </si>
-  <si>
-    <t>infrequent_standing: 두 발로 서는 경우가 거의 없어요.
-prevent_standing: 서자마자 바로 안아주는 등 최대한 두 발로 서지 못하게 해요.
-indifferent: 별로 신경 쓰지 않아요.</t>
-  </si>
-  <si>
-    <t>최근 반려인님을 피하거나 숨는 경우가 있었나요?</t>
-  </si>
-  <si>
-    <t>normal: 거의 숨지 않아요.
-occasional: 가끔 그래요.
-increased: 최근에 심해졌어요.
-constant: 늘 숨어있고, 손길을 피해요.</t>
-  </si>
-  <si>
     <t>cat</t>
-  </si>
-  <si>
-    <t>반려인님이 외출하고 집에 돌아오면 어떻게 행동하나요?</t>
   </si>
   <si>
     <t>friendly: 친근하게 반겨줘요.
@@ -398,111 +141,13 @@
 fearful: 도망가거나 숨어있어요.</t>
   </si>
   <si>
-    <t>평소 모르는 사람을 보면 어떻게 행동하나요?</t>
-  </si>
-  <si>
-    <t>sociable: 친근하게 다가가요.
-avoidant: 도망가거나 숨어있어요.
-defensive_aggressive: 방어 태세를 취하거나, 때로는 공격성을 보여요.
-indifferent: 사람에게 별로 관심이 없어요.</t>
-  </si>
-  <si>
     <t>주로 생활하는 공간은 어디인가요?</t>
   </si>
   <si>
-    <t>주로 생활하는 환경에 외부인의 출입이 잦은 편인가요?</t>
-  </si>
-  <si>
-    <t>high_different_visitors: 네, 매번 다른 외부인이 자주 방문해요.
-high_repeated_visitors: 네, 그런데 대부분 여러 번 방문한 친구들이에요.
-low_recent_increase: 아니요, 그런데 최근 수리 기사님 등의 방문이 잦았어요.
-low_family_only: 아니요, 가족들만 출입해요.</t>
-  </si>
-  <si>
-    <t>캣타워 또는 올라갈 수 있는 높은 가구가 있나요?</t>
-  </si>
-  <si>
-    <t>최근 놀다가 갑자기 멈추거나 휴식을 취하는 경우가 있었나요?</t>
-  </si>
-  <si>
-    <t>high: 아니요, 집사가 먼저 지칠 때 까지 멈추지 않고 놀아요.
-moderate: 대부분 지치지 않고 잘 놀지만, 일주일에 1-2회 정도는 먼저 놀이를 멈추거나 쉬고 싶어해요.
-low: 일주일에 3-4회 정도 먼저 놀이를 멈추거나 쉬고 싶어해요.
-very_low: 대부분 먼저 놀이를 멈추거나 쉬고 싶어해요.</t>
-  </si>
-  <si>
-    <t>ready: 좋아요! 답변할게요.
-difficult: 지금은 어려워요.</t>
-  </si>
-  <si>
-    <t>현재 기준으로 {@petname}의 눈이 충혈되어있나요?</t>
-  </si>
-  <si>
-    <t>normal: 아니요, 안 그래요.
-mild_congestion: 약간 충혈되어있어요.
-severe_congestion: 심하게 충혈되어있어요.</t>
-  </si>
-  <si>
-    <t>현재 {@petname}의 동공 표면이 뿌옇거나 하얀색으로 보이는 부분이 있나요?</t>
-  </si>
-  <si>
-    <t>cloudy: 네.
-clear: 아니요.</t>
-  </si>
-  <si>
-    <t>현재 기준으로 코가 촉촉한가요?</t>
-  </si>
-  <si>
-    <t>moist: 네.
-moist_with_discharge: 네, 그런데 하얗거나 노란 콧물을 동반하고 있어요.
-dry: 아니요, 건조해요.</t>
-  </si>
-  <si>
-    <t>현재 기준으로 잇몸은 촉촉한가요?</t>
-  </si>
-  <si>
-    <t>moist: 네, 촉촉해요.
-dry: 아니요, 건조해요.
-unknown: 입안을 안 보여줘서 확인하기 어려워요.</t>
-  </si>
-  <si>
     <t>현재 귓구멍 내부는 어떤 상태인가요?</t>
   </si>
   <si>
-    <t>normal: 정상 같아 보여요.
-light_yellow_earwax: 연노랑색 귀지가 많아요.
-brown_earwax: 갈색 귀지가 많아요.
-narrowed_earhole: 귀지 여부와 상관 없이 귓구멍이 좁아진 것 같아요.
-reddened: 최근 많이 긁어서인지 붉게 충혈됐어요.
-unconfirmed: 보여주지 않아서 확인이 불가능해요.</t>
-  </si>
-  <si>
-    <t>방금 답변해 주신 증상이 양쪽 모두에서 나타나나요?</t>
-  </si>
-  <si>
-    <t>bilateral: 네.
-unilateral: 아니요.</t>
-  </si>
-  <si>
-    <t>현재 피부에 상처 또는 염증이 있는 상태인가요?</t>
-  </si>
-  <si>
     <t>털에 윤기가 있나요?</t>
-  </si>
-  <si>
-    <t>clumped: 네, 그런데 뭉칠 정도로 엉겨 붙어있어요.
-shiny: 네, 적당하게 윤기가 보여요.
-dull: 아니요, 푸석해 보여요.</t>
-  </si>
-  <si>
-    <t>{@petname}에게 탈모 증상이 있나요?</t>
-  </si>
-  <si>
-    <t>no_symptoms: 아니요.
-localized: 네, 한 곳에서만 털이 빠져요.
-symmetrical: 네, 대칭적으로 여러 곳에서 빠지고 있어요.
-asymmetrical: 네, 비대칭적으로 여러 곳에서 빠지고 있어요.
-generalized: 네, 전신적으로 빠지고 있어요.</t>
   </si>
   <si>
     <t>시간을 내어 이 설문조사에 참여해 주셔서 감사합니다.
@@ -538,17 +183,7 @@
     <t>Design</t>
   </si>
   <si>
-    <t xml:space="preserve">주로 어떤 사료를 먹나요?
-</t>
-  </si>
-  <si>
     <t>두 가지 이상의 사료를 먹는다면, 가장 많은 비중을 차지하는 사료를 기준으로 선택해주세요.</t>
-  </si>
-  <si>
-    <t>처방 사료를 먹는다면, 어떤 사료인가요?</t>
-  </si>
-  <si>
-    <t>두 가지 이상의 간식을 먹는다면, 가장 많은 비중을 차지하는 간식 기준으로 선택해주세요.</t>
   </si>
   <si>
     <t>주로 어떤 간식을 먹나요?</t>
@@ -558,17 +193,6 @@
 </t>
   </si>
   <si>
-    <t>권장되는 하루 간식 복용량은 하루에 먹는 사료량의 10% 이하입니다.</t>
-  </si>
-  <si>
-    <t>지금부터는 관찰이 필요해요. 답변을 이어가시겠어요?</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;
-만약 코의 촉촉함, 귓구멍 상태 등을 안다면 이어서 답변할 수 있어요:)&lt;br&gt;
-답변이 많을수록 더 정교한 진단 결과를 받을 수 있어요.</t>
-  </si>
-  <si>
     <t>SET(@booster_vaccination)
 IF(@gender==female) THEN (GOTO: 3) ELSE (GOTO: 6)</t>
   </si>
@@ -582,9 +206,6 @@
     <t>SET(@treat_intake)</t>
   </si>
   <si>
-    <t>SET(@constipation)</t>
-  </si>
-  <si>
     <t>SET(@water_intake_change)</t>
   </si>
   <si>
@@ -725,63 +346,6 @@
   <si>
     <t>SET(@toothbrushing)
 IF(@target==cat) THEN (GOTO: 31) ELSE (GOTO: 32)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">none: 간식은 주지 않아요.
-wet_snacks: 습식 간식류 (츄르, 양갱, 퓨레, 무스, 동물용 통조림 등)
-dry_snacks: 건식 간식류 (동결건조, 쿠키, 육포, 저키 등)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>functional_snacks: 기능성 간식류 (오메가3, 유산균 등 특정 건강 보조성분이 포함된 간식류)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>dog_dental_chew: 개껌류</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-natural_fruit_vegetable: 천연 재료 간식류 중 과일, 야채 위주
-natural_meat: 천연 재료 간식류 중 살코기, 닭가슴살, 황태포 등 육류 위주
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>others: 기타 (아래에 작성해 주세요.)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -817,15 +381,93 @@
 IF(@grooming==regular) THEN (GOTO:23) ELSE (GOTO:25)</t>
   </si>
   <si>
+    <t>common
+female</t>
+  </si>
+  <si>
+    <t>common
+cat</t>
+  </si>
+  <si>
+    <t>common
+treat</t>
+  </si>
+  <si>
+    <t>common
+dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">common
+</t>
+  </si>
+  <si>
+    <t>SET(@observation)
+IF(@observation==difficult) THEN (GOTO:62) ELSE (GOTO:53)</t>
+  </si>
+  <si>
+    <t>SET(@urine_odor)
+IF(@target==cat) THEN (GOTO: 20) ELSE (GOTO:21)</t>
+  </si>
+  <si>
+    <t>yes: 네, 매달 예방하고 있어요.
+no: 아니오, 매달 예방하지 않아요.</t>
+  </si>
+  <si>
+    <t>yes: 네, 추가 접종하고 있어요.
+conditional: 항제가검사를 통해 필요한 추가 접종만 진행하고 있어요.
+no: 아니오, 추가 접종하지 않아요.</t>
+  </si>
+  <si>
+    <t>yes: 현재 임신 중.
+no: 해당 없음.</t>
+  </si>
+  <si>
+    <t>yes: 출산한 적 있음.
+no: 해당 없음</t>
+  </si>
+  <si>
+    <t>yes: 현재 수유 중.
+no: 해당 없음</t>
+  </si>
+  <si>
+    <t>decreased_significantly: 눈에 띄게 줄었어요.
+decreased_slightly: 조금 줄었어요.
+no_change: 비슷해요.
+increased_slightly: 조금 늘었어요.
+increased_significantly: 눈에 띄게 늘었어요.</t>
+  </si>
+  <si>
+    <t>고양이 헤르페스 바이러스 감염 증상(재채기, 콧물, 결막염 등)이 현재 있나요?</t>
+  </si>
+  <si>
+    <t>positive: 네, 증상이 있어요.
+negative: 아니오, 증상이 없어요.
+carrier: 증상은 없지만, 보균자예요.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">주로 어떤 사료를 먹이나요?
+</t>
+  </si>
+  <si>
+    <t>animal_protein: 동물성 단백질 일반 사료 (곤충 단백질 포함)
+plant_protein: 식물성 단백질 일반 사료&lt;br&gt;(두부, 콩 단백질 등이 포함돼요.)
+prescription_diet: 수의사 처방 사료&lt;br&gt;(Royal Canin, Hill's, Purina, Velixer 등에서 생산한 처방식을 이야기해요.)
+cooked_meat: 화식류 제품&lt;br&gt;(기성 제품 또는 집에서 직접 굽는 등 조리한 고기 등이 포함돼요.)
+raw_diet: 생식 및 동결건조 사료&lt;br&gt;(조리 안 된 어류, 육류 등이 포함돼요.)</t>
+  </si>
+  <si>
+    <t>무슨 목적의 처방 사료인가요?</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">weight_control: 비만 예방 및 체중 감량 사료
-renal: 신장 (Renal, Kidney)
-urinary: 비뇨기계 (Urinary, 결석 예방 사료)
-hepatic: 간 (Hepatic, Liver)
-hypoallergic: 저알러지 (Hypoallergic, 가수분해 사료)
-intestinal: 소화기계 (Intearinal, Microbiome)
-cardiac: 심장 (Cardiac, Heart)
-recovery: 회복용 처방사료 (A/D 또는 P/D 또는 Recovery)
+      <t xml:space="preserve">weight_control: 비만 예방 및 체중 감량
+renal: 신장 건강
+urinary: 비뇨기계 건강(결석 예방)
+hepatic: 간 건강
+hypoallergic: 알러지 예방
+intestinal: 소화기계 건강
+cardiac: 심장 건강
+recovery: 회복용 처방 사료
 </t>
     </r>
     <r>
@@ -835,45 +477,32 @@
         <color rgb="FF7030A0"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>other: 기타 처방사료 (아래에 작성해 주세요.)</t>
+      <t>other: 직접 작성하기</t>
     </r>
   </si>
   <si>
-    <t>common
-female</t>
-  </si>
-  <si>
-    <t>common
-cat</t>
-  </si>
-  <si>
-    <t>common
-treat</t>
-  </si>
-  <si>
-    <t>common
-dog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">common
+    <r>
+      <t xml:space="preserve">none: 간식을 먹지 않아요.
+wet_snacks: 습식 간식류&lt;br&gt;(츄르, 양갱, 퓨레, 무스, 동물용 통조림 등이 있어요.)
+dry_snacks: 건식 간식류&lt;br&gt;(동결건조, 쿠키, 육포, 저키 등이 있어요.)
 </t>
-  </si>
-  <si>
-    <t>SET(@observation)
-IF(@observation==difficult) THEN (GOTO:62) ELSE (GOTO:53)</t>
-  </si>
-  <si>
-    <t>SET(@ear_condition)
-IF((@ear_condition!=normal) AND (@ear_condition!=unconfirmed)) THEN (GOTO:58) ELSE (GOTO:59)</t>
-  </si>
-  <si>
-    <t>SET(@urine_odor)
-IF(@target==cat) THEN (GOTO: 20) ELSE (GOTO:21)</t>
-  </si>
-  <si>
+    </r>
     <r>
-      <t xml:space="preserve">indoor: 실내 - 아파트, 빌라, 주택 등 (실내에서만 생활해요. 외출하지 않아요.)
-outdoor: 실외 - 마당냥이 혹은 길냥이 등 (자유롭게 외출할 수 있어요.)
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>functional_snacks: 기능성 간식류&lt;br&gt;(오메가3, 유산균 등 특정한 건강보조성분이 포함된 간식류를 말해요.)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -883,15 +512,448 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>other: 기타 (아래에 작성해 주세요.)</t>
+      <t>IF(@type==dog) THEN (dog_dental_chew: 개껌류)</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+natural_fruit_vegetable: 천연 재료 간식류 중 과일, 야채 위주
+natural_meat: 천연 재료 간식류 중 육류 위주
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>other: 직접 작성하기</t>
+    </r>
+  </si>
+  <si>
+    <t>recommended_or_less: 권장량만큼 주거나, 적게 줘요.
+more_than_recommended: 권장량보다 많이 줘요.</t>
+  </si>
+  <si>
+    <t>fast: 주자마자 순식간에 잘 씹지 않고 삼켜요.
+moderate: 적당한 속도로 잘 씹어서 먹어요.
+slow: 느리게 먹거나, 큰 관심이 없어 보여요.</t>
+  </si>
+  <si>
+    <t>최근 구토 또는 역류 증상이 있었나요?</t>
+  </si>
+  <si>
+    <t>absent: 아니요.
+intermittent: 네, 종종 있어요.
+increased_recently: 최근 들어 심해졌어요.</t>
+  </si>
+  <si>
+    <t>dry_hard: 건조하고 딱딱해요.
+dry_soft: 건조한 편이지만, 말랑해요.
+moist_soft: 습기가 있으면서 적당히 말랑해요. 항문 주변에 살짝 묻어날 때도 있어요.
+loose: 변이 물러요. 항문 주변에 많이 묻어나요.
+diarrhea : 설사를 해요.</t>
+  </si>
+  <si>
+    <r>
+      <t>SET(@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>constipation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>no: 아니오, 변비는 없어요.
+recent: 네, 최근에 변비가 생겼어요.
+chronic: 예전부터 변비가 있었어요.</t>
+  </si>
+  <si>
+    <t>최근 음수량에 변화가 있었나요?</t>
+  </si>
+  <si>
+    <t>최근 소변 횟수에 변화가 있었나요?</t>
+  </si>
+  <si>
+    <t>최근 6개월 내에 곰팡이, 세균 등에 의한 감염성 피부염이 2회 이상 발생했나요?</t>
+  </si>
+  <si>
+    <t>주로 생활하는 실내가 건조한가요?</t>
+  </si>
+  <si>
+    <t>입 안에 염증이 있거나 안 좋은 냄새가 나나요? 만약 그렇다면 더 심해졌나요?</t>
+  </si>
+  <si>
+    <t>치아 관리를 어떻게 하고 있나요?</t>
+  </si>
+  <si>
+    <t>최근 기침이나 재채기를 했나요?</t>
+  </si>
+  <si>
+    <t>최근 눈에 띄는 성격 변화가 있었나요?</t>
+  </si>
+  <si>
+    <t>캣타워나 높은 가구가 있나요?</t>
+  </si>
+  <si>
+    <t>최근 노는 도중에 갑자기 멈추거나 휴식을 취하는 경우가 있었나요?</t>
+  </si>
+  <si>
+    <t>산책은 어느 정도로 하나요?</t>
+  </si>
+  <si>
+    <t>산책할 때, 다리가 불편해 보이나요?</t>
+  </si>
+  <si>
+    <t>미끄럼 방지 제품을 사용하시나요?</t>
+  </si>
+  <si>
+    <t>지금부터는 관찰이 필요해요. 답변을 한다면, 더 정교한 결과를 받을 수 있어요.</t>
+  </si>
+  <si>
+    <t>ready: 좋아요, 이어서 할게요!
+difficult: 지금은 어려워요.</t>
+  </si>
+  <si>
+    <t>귓구멍의 증상이 양 쪽에서 나타나나요?</t>
+  </si>
+  <si>
+    <t>탈모 증상이 있나요?</t>
+  </si>
+  <si>
+    <t>decreased: 음수량이 줄었어요.
+stable: 음수량이 그대로예요.
+increase: 음수량이 늘었어요.</t>
+  </si>
+  <si>
+    <t>decreased: 소변량이 줄었어요.
+stable: 소변량이 그대로예요.
+increased: 소변량이 늘었어요.</t>
+  </si>
+  <si>
+    <t>decreased: 소변 횟수가 줄었어요.
+stable: 소변 횟수가 그대로예요.
+increased: 소변 횟수가 늘었어요.</t>
+  </si>
+  <si>
+    <t>normal: 아니오, 그대로예요.
+strong: 네, 소변 냄새가 심해졌어요.</t>
+  </si>
+  <si>
+    <t>decreased: 화장실 방문을 평소보다 덜 해요.
+stable: 평소와 비슷하게 화장실을 방문해요.
+increased: 화장실 방문을 평소보다 자주 해요.</t>
+  </si>
+  <si>
+    <t>no_bathing: 목욕을 안 해요.
+less_than_monthly: 월에 1회 목욕해요.
+biweekly: 2주에 1회 목욕해요.
+weekly: 1주에 1회 목욕해요.
+twice_weekly: 1주에 2회 목욕해요.
+more_than_twice_weekly: 1주에 3회 이상 목욕해요.</t>
+  </si>
+  <si>
+    <t>regular:네, 주기적으로 미용해요.
+not_regular: 아니오, 주기적으로 미용하지 않아요.</t>
+  </si>
+  <si>
+    <t>home: 집에서 직접 미용해요.
+shop_or_vet: 샵이나 병원에서 미용해요.</t>
+  </si>
+  <si>
+    <t>yes: 네, 마취해요.
+no: 아니오, 마취하지 않아요.</t>
+  </si>
+  <si>
+    <t>yes: 네, 2회 이상 발생했어요.
+no: 아니오, 2회 이상 발생하지 않았어요.</t>
+  </si>
+  <si>
+    <t>not_dry: 건조해서 가습기를 틀어놔요.
+humid: 건조하지 않아요.
+dry_with_humidifier: 습한 편이에요.
+dry_without_care: 건조한 편이지만 특별히 신경 쓰고 있지 않아요.</t>
+  </si>
+  <si>
+    <t>never: 아니요, 그렇지 않아요.
+1-2_times_weekly: 주에 1~2회 드물게 보여요.
+3-5_times_weekly: 주에 3~5회 종종 보여요.
+daily: 거의 매일 보여요.</t>
+  </si>
+  <si>
+    <t>absent: 염증이나 구취가 없어요.
+present: 염증은 있지만, 구취가 심해지지 않았어요.
+worsened: 염증이 있고, 구취가 전보다 심해졌어요.
+unconfirmed: 입 안을 안 보여줘서 확인이 어려워요.</t>
+  </si>
+  <si>
+    <t>가장 최근 스케일링은 언제인가요?</t>
+  </si>
+  <si>
+    <t>last_6_months: 6개월 내에 스케일링을 받았어요.
+6_months_to_1_year: 6개월~1년 사이에 스케일링을 받았어요.
+over_1_year_or_never: 받은지 1년이 넘었거나, 받은 적이 없어요.</t>
+  </si>
+  <si>
+    <t>everyday:매일 칫솔질을 해요.
+3_times_weekly: 주에 3회 이상 칫솔질을 해요.
+only_toothpaste: 치약을 잇몸과 치아에 발라주거나, 마시는 물에 치석 방지 제품을 섞어주기만 해요.
+never: 잘 해주지 않고 있어요.</t>
+  </si>
+  <si>
+    <t>yes: 네, 그런 경우가 있어요.
+no: 아니오, 그렇지 않아요.</t>
+  </si>
+  <si>
+    <t>never: 아니오, 그렇지 않아요.
+1-2_times_weekly: 주에 1~2회 비정상적인 숨소리를 내요.
+3-5_times_weekly: 주에 3~5회 비정상적인 숨소리를 내요.
+daily: 매일 비정상적인 숨소리를 내요.</t>
+  </si>
+  <si>
+    <t>none: 아니오, 그렇지 않아요.
+occasional: 운동을 격하게 했거나, 많이 흥분했을 때에만 캑캑거려요.
+frequent: 특별한 일이 없어도 캑캑거리는 모습이 하루에 한두 번 가끔 보여요.
+very_frequent: 특별한 일이 없어도 캑캑거리는 모습이 하루에 3~5회 이상 자주 보여요.</t>
+  </si>
+  <si>
+    <t>excitable: 항상 흥분한 상태예요.
+calm_excitable: 때로는 격하지만, 평소에는 차분한 편이에요.
+peaceful_expressive: 꼬리를 살랑이거나 만져달라고 오는 등 평온한 방식으로 기분과 상태를 표현해요.
+indifferent: 주변 환경 변화에 예민한 편은 아니에요. 성격이 무던해요.
+anxious_sensitive: 겁이 많고, 반려인과 멀어지거나 환경이 변화하면 많이 불안해하고 예민한 편이에요.</t>
+  </si>
+  <si>
+    <t>immediate_barking: 나가자마자 짖기 시작해요.
+occasional_barking: 나간 직후는 아니지만, 종종 짖기도 해요.
+indifferent: 크게 신경쓰지 않아 해요.</t>
+  </si>
+  <si>
+    <t>none: 산책을 거의 하지 않고, 활동량이 적어요.
+short: 하루에 30분 이내로 산책해요.
+medium: 하루에 30분 이상 60분 이내로 산책해요.
+long: 하루에 1시간 이상씩 산책해요.
+indoor: 산책을 자주 안 가지만, 실내 활동량이 많아요.</t>
+  </si>
+  <si>
+    <t>no_symptoms: 아니요, 그렇지 않아요.
+unstable_after_short_walk: 조금만 걸어도 다리를 떨거나 절뚝이는 등 불안정해 보여요.
+unstable_after_long_walk: 오래 걸으면 다리를 떨거나 절뚝이는 등 불안정해 보여요.</t>
+  </si>
+  <si>
+    <t>slippery: 대리석 같이 미끄러운 바닥
+less_slippery: 나무 바닥 같이 조금 덜 미끄러운 바닥
+non_slippery: 장판 같이 미끄러짐이 거의 없는 바닥</t>
+  </si>
+  <si>
+    <t>low: 좌식 생활을 하는 중이거나, 소파나 침대가 낮은 편이에요.
+high: 소파나 침대가 높은 편이에요.
+high_stepped: 소파나 침대가 높은 편이지만, 계단식 구조물이 함께 있어요.</t>
+  </si>
+  <si>
+    <t>runs_and_jumps: 달려와서 점프해요.
+requests_assistance: 올려달라고 애원해요.
+uses_stairs_or_objects: 계단이나 주변 사물을 이용해서 올라와요.
+avoids_climbing: 잘 올라오지 않아요.</t>
+  </si>
+  <si>
+    <t>infrequent_standing: 두 발로 거의 서지 않아요.
+prevent_standing: 서자마자 바로 안아주거나 지시하는 등 최대한 두 발로 서지 않게 해요.
+indifferent: 크게 신경쓰지 않아요.</t>
+  </si>
+  <si>
+    <t>normal: 거의 숨지 않아요.
+occasional: 가끔 숨어요.
+increased: 최근에 더 숨는 편이에요.
+constant: 늘 숨고, 손길을 피해요.</t>
+  </si>
+  <si>
+    <t>sociable: 친근하게 다가가요.
+avoidant: 도망가거나 숨어요.
+defensive_aggressive: 방어 태세를 취하거나, 공격성을 보여요.
+indifferent: 사람에게 큰 관심이 없어요.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">indoor: 실내에서만 생활하고 외출하지 않아요.
+outdoor: 자유롭게 외출할 수 있어요.&lt;br&gt;(마당냥이나 길냥이를 포함해요.)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>other: 직접 작성하기</t>
+    </r>
+  </si>
+  <si>
+    <t>high_different_visitors: 네, 다른 외부인이 자주 방문해요.
+high_repeated_visitors: 네, 여러 번 왔던 외부인이 자주 방문해요.
+low_recent_increase: 아니오, 최근에만 외부인의 방문이 잦았어요.
+low_family_only: 아니오, 가족들만 출입해요.</t>
+  </si>
+  <si>
+    <t>yes: 네, 높은 가구가 있어요.
+no: 아니오, 높은 가구가 없어요.</t>
+  </si>
+  <si>
+    <t>high: 아니오, 집사가 지칠 때까지 계속 놀아요.
+moderate: 보통 지치지 않고 잘 놀지만, 주에 1~2회는 먼저 놀이를 멈추거나 쉬고 싶어 해요.
+low: 주에 3~4회 먼저 놀이를 멈추거나 쉬고 싶어 해요.
+very_low: 대부분 먼저 놀이를 멈추거나 쉬고 싶어 해요.</t>
+  </si>
+  <si>
+    <t>moist: 네, 잇몸이 촉촉해요.
+dry: 아니오, 잇몸이 건조해요.
+unknown: 보여주지 않아 확인하기 어려워요.</t>
+  </si>
+  <si>
+    <t>normal: 아니오, 충혈되지 않았어요.
+mild_congestion: 네, 약간 충혈되어 있어요.
+severe_congestion: 네, 심하게 충혈되어 있어요.</t>
+  </si>
+  <si>
+    <t>cloudy: 네, 그런 부분이 있어요.
+clear: 아니오, 그렇지 않아요.</t>
+  </si>
+  <si>
+    <t>moist: 네, 코가 촉촉해요.
+moist_with_discharge: 네, 그런데 하얗거나 노란 콧물을 동반하고 있어요.
+dry: 아니오, 코가 건조해요.</t>
+  </si>
+  <si>
+    <t>normal: 정상처럼 보여요.
+light_yellow_earwax: 연노란색 귀지가 많아요.
+brown_earwax: 갈색 귀지가 많아요.
+narrowed_earhole: 귀지 여부와 상관 없이 귓구멍이 좁아진 것처럼 보여요.
+reddened: 붉게 충혈됐어요.
+unconfirmed: 보여주지 않아 확인하기 어려워요.</t>
+  </si>
+  <si>
+    <t>bilateral: 네, 양 쪽 모두에서 나타나요.
+unilateral: 아니오, 한 쪽에서만 나타나요.</t>
+  </si>
+  <si>
+    <t>yes: 네, 있어요.
+no: 아니오, 없어요.</t>
+  </si>
+  <si>
+    <t>clumped: 네, 하지만 뭉치고 영겨 있어요.
+shiny: 네, 적당히 윤기가 있고 매끄러워요.
+dull: 아니오, 푸석해요.</t>
+  </si>
+  <si>
+    <t>no_symptoms: 아니오, 탈모 증상은 없어요.
+localized: 네, 한 곳에서만 털이 빠져요.
+symmetrical: 네, 대칭적으로 여러 곳에서 빠져요.
+asymmetrical: 네, 비대칭적으로 여러 곳에서 빠져요.
+generalized: 네, 전신에서 털이 빠져요.</t>
+  </si>
+  <si>
+    <t>두 가지 이상의 간식을 먹는다면, 가장 많은 비중을 차지하는 간식을 기준으로 선택해주세요.</t>
+  </si>
+  <si>
+    <t>*권장 하루 간식 복용량: 하루 사료량의 10% 이하</t>
+  </si>
+  <si>
+    <t>아이의 눈, 코, 귓구멍, 털의 상태와 상처 여부를 안다면 이어서 답변할 수 있어요. (총 8~9문항)</t>
+  </si>
+  <si>
+    <t>현재 {@petname}이 임신 중인가요?</t>
+  </si>
+  <si>
+    <t>최근 {@petname}에게 변비 증상이 있었나요?</t>
+  </si>
+  <si>
+    <t>최근 {@petname}의 화장실 방문 빈도에 변화가 있었나요?</t>
+  </si>
+  <si>
+    <t>최근 {@petname}이 눈을 반복적으로 비비는 행동을 보인 적이 있나요?</t>
+  </si>
+  <si>
+    <t>반려인 님이 집을 비울 때, {@petname}은 어떻게 행동하나요?</t>
+  </si>
+  <si>
+    <t>소파, 침대 등 높은 곳을 오르내릴 때, {@petname}은 어떻게 행동하나요?</t>
+  </si>
+  <si>
+    <t>최근 {@petname}이 반려인 님을 피하거나 숨은 적이 있었나요?</t>
+  </si>
+  <si>
+    <t>반려인 님이 외출하고 집에 돌아오면, {@petname}은 어떻게 행동하나요?</t>
+  </si>
+  <si>
+    <t>평소 모르는 사람을 보면 {@petname}은 어떻게 행동하나요?</t>
+  </si>
+  <si>
+    <t>현재 기준으로 {@petname}의 눈이 충혈되어 있나요?</t>
+  </si>
+  <si>
+    <t>현재 {@petname}의 동공 표면에 뿌옇거나 하얗게 보이는 부분이 있나요?</t>
+  </si>
+  <si>
+    <t>현재 기준으로 {@petname}의 코가 촉촉한가요?</t>
+  </si>
+  <si>
+    <t>현재 기준으로 {@petname}의 잇몸이 촉촉한가요?</t>
+  </si>
+  <si>
+    <t>현재 {@petname}의 피부에 상처 또는 염증이 있는 상태인가요?</t>
+  </si>
+  <si>
+    <t>pad_used: 미끄럼 방지 패드 사용 중
+cream_used: 미끄럼 방지 크림 사용 중
+both_used: 미끄럼 방지 패드, 크림 둘 다 사용 중
+none_used: 아무 것도 사용하지 않음</t>
+  </si>
+  <si>
+    <t>SET(@ear_condition)
+IF(@ear_condition==normal) THEN (GOTO:59)
+ELIF(@ear_condition==unconfirmed) THEN (GOTO:59)
+GOTO:58</t>
+  </si>
+  <si>
+    <t>{@petname}이 주로 생활하는 환경에 외부인의 출입이 잦은 편인가요?</t>
+  </si>
+  <si>
+    <t>{@petname}이 주로 생활하는 실내 공간의 바닥은 어떤가요?</t>
+  </si>
+  <si>
+    <t>{@petname}이 주로 생활하는 실내 공간의 가구 높이는 어떤가요?</t>
+  </si>
+  <si>
+    <t>{@petname}이 두 발로 서려고 할 때, 반려인 님은 어떻게 반응하시나요?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -930,8 +992,21 @@
       <color rgb="FF7030A0"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -968,6 +1043,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -978,10 +1059,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1042,8 +1124,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1358,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5C60D7-EAD3-EB46-856C-21C3EE23727A}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1367,11 +1463,12 @@
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="42.5" style="7" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
-    <col min="4" max="4" width="69.83203125" customWidth="1"/>
-    <col min="5" max="5" width="63" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="84.33203125" customWidth="1"/>
+    <col min="5" max="5" width="56.83203125" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="7" max="7" width="3.5" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1391,10 +1488,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>124</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -1411,10 +1508,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
@@ -1422,7 +1519,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.2">
@@ -1430,16 +1527,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>134</v>
+        <v>47</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -1447,7 +1544,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1455,16 +1552,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>187</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>176</v>
+        <v>88</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1472,7 +1569,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1480,16 +1577,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>175</v>
+        <v>87</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1497,7 +1594,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1505,16 +1602,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1522,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -1530,16 +1627,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -1547,7 +1644,7 @@
         <v>3</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
@@ -1555,16 +1652,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -1572,7 +1669,7 @@
         <v>3</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="133" customHeight="1" x14ac:dyDescent="0.2">
@@ -1580,26 +1677,26 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="18">
         <v>3</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.2">
@@ -1607,26 +1704,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>121</v>
+        <v>40</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18">
         <v>3</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="11" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.2">
@@ -1634,26 +1731,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>129</v>
+        <v>45</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>184</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="11">
         <v>3</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1661,26 +1758,26 @@
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>137</v>
+        <v>50</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>131</v>
+        <v>185</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18">
         <v>3</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>190</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.2">
@@ -1688,16 +1785,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -1705,7 +1802,7 @@
         <v>3</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1713,16 +1810,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>135</v>
+        <v>48</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -1730,7 +1827,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="104" customHeight="1" x14ac:dyDescent="0.2">
@@ -1738,16 +1835,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>177</v>
+        <v>89</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -1755,7 +1852,7 @@
         <v>3</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="49" customHeight="1" x14ac:dyDescent="0.2">
@@ -1763,16 +1860,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1780,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1788,16 +1885,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -1805,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1813,16 +1910,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>178</v>
+        <v>90</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -1830,7 +1927,7 @@
         <v>3</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -1838,16 +1935,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>33</v>
+        <v>144</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1855,24 +1952,24 @@
         <v>3</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="6" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>36</v>
+        <v>145</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>195</v>
+        <v>104</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -1880,7 +1977,7 @@
         <v>3</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -1888,16 +1985,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>37</v>
+        <v>189</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>33</v>
+        <v>146</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>185</v>
+        <v>96</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -1905,7 +2002,7 @@
         <v>3</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -1913,16 +2010,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>39</v>
+        <v>147</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1930,24 +2027,24 @@
         <v>4</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <v>22</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>41</v>
+        <v>148</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -1955,24 +2052,24 @@
         <v>4</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <v>23</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -1980,7 +2077,7 @@
         <v>4</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1988,16 +2085,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -2005,7 +2102,7 @@
         <v>4</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2013,16 +2110,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>141</v>
+        <v>53</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -2030,32 +2127,32 @@
         <v>4</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="30" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="28">
         <v>26</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="18">
+      <c r="B27" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="30">
         <v>4</v>
       </c>
-      <c r="I27" s="16" t="s">
-        <v>9</v>
+      <c r="I27" s="28" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -2063,16 +2160,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>48</v>
+        <v>190</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>49</v>
+        <v>153</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>143</v>
+        <v>55</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
@@ -2080,7 +2177,7 @@
         <v>4</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.2">
@@ -2088,16 +2185,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>51</v>
+        <v>154</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>144</v>
+        <v>56</v>
       </c>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -2105,7 +2202,7 @@
         <v>4</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -2113,16 +2210,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>52</v>
+        <v>155</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>53</v>
+        <v>156</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -2130,7 +2227,7 @@
         <v>4</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="89" customHeight="1" x14ac:dyDescent="0.2">
@@ -2138,16 +2235,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>55</v>
+        <v>157</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
@@ -2155,7 +2252,7 @@
         <v>4</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2163,16 +2260,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>8</v>
+        <v>158</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
@@ -2180,7 +2277,7 @@
         <v>4</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>189</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.2">
@@ -2188,16 +2285,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>147</v>
+        <v>59</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
@@ -2205,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>192</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.2">
@@ -2213,16 +2310,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>149</v>
+        <v>61</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -2230,24 +2327,24 @@
         <v>4</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="116" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>61</v>
+      <c r="B35" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>62</v>
+        <v>161</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>148</v>
+        <v>60</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -2255,7 +2352,7 @@
         <v>5</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="85" customHeight="1" x14ac:dyDescent="0.2">
@@ -2263,16 +2360,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>150</v>
+        <v>62</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2280,7 +2377,7 @@
         <v>5</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.2">
@@ -2288,16 +2385,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>66</v>
+        <v>191</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2305,7 +2402,7 @@
         <v>5</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.2">
@@ -2313,16 +2410,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>69</v>
+        <v>163</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2330,7 +2427,7 @@
         <v>5</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -2338,16 +2435,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>153</v>
+        <v>65</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2355,7 +2452,7 @@
         <v>5</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.2">
@@ -2363,16 +2460,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>73</v>
+        <v>164</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -2380,24 +2477,24 @@
         <v>5</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="22">
         <v>40</v>
       </c>
-      <c r="B41" s="23" t="s">
-        <v>74</v>
+      <c r="B41" s="26" t="s">
+        <v>204</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>75</v>
+        <v>165</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>155</v>
+        <v>67</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
@@ -2405,7 +2502,7 @@
         <v>5</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -2413,16 +2510,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>76</v>
+        <v>137</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>77</v>
+        <v>201</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2430,24 +2527,24 @@
         <v>5</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>78</v>
+      <c r="B43" s="26" t="s">
+        <v>205</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>79</v>
+        <v>166</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2455,7 +2552,7 @@
         <v>5</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="83" customHeight="1" x14ac:dyDescent="0.2">
@@ -2463,16 +2560,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>80</v>
+        <v>192</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2480,24 +2577,24 @@
         <v>5</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>82</v>
+      <c r="B45" s="26" t="s">
+        <v>206</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>159</v>
+        <v>71</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -2505,7 +2602,7 @@
         <v>5</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="15" customFormat="1" ht="68" x14ac:dyDescent="0.2">
@@ -2513,16 +2610,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>84</v>
+        <v>193</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
@@ -2530,7 +2627,7 @@
         <v>6</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2538,16 +2635,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>87</v>
+        <v>194</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
@@ -2555,7 +2652,7 @@
         <v>6</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="15" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -2563,16 +2660,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>89</v>
+        <v>195</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
@@ -2580,7 +2677,7 @@
         <v>6</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="21" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
@@ -2588,16 +2685,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>163</v>
+        <v>75</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
@@ -2605,24 +2702,24 @@
         <v>6</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="15" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="13">
         <v>49</v>
       </c>
-      <c r="B50" s="14" t="s">
-        <v>92</v>
+      <c r="B50" s="27" t="s">
+        <v>203</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
@@ -2630,7 +2727,7 @@
         <v>6</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2638,16 +2735,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
@@ -2655,7 +2752,7 @@
         <v>6</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="15" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
@@ -2663,16 +2760,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>96</v>
+        <v>174</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>166</v>
+        <v>78</v>
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
@@ -2680,7 +2777,7 @@
         <v>6</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="12" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -2688,26 +2785,26 @@
         <v>52</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>193</v>
+        <v>103</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>133</v>
+        <v>186</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="18">
         <v>7</v>
       </c>
       <c r="I53" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="12" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -2715,16 +2812,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>98</v>
+        <v>196</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>99</v>
+        <v>176</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
       <c r="F54" s="16"/>
       <c r="G54" s="16"/>
@@ -2732,7 +2829,7 @@
         <v>7</v>
       </c>
       <c r="I54" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="12" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2740,16 +2837,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>100</v>
+        <v>197</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>101</v>
+        <v>177</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="F55" s="16"/>
       <c r="G55" s="16"/>
@@ -2757,7 +2854,7 @@
         <v>7</v>
       </c>
       <c r="I55" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="12" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.2">
@@ -2765,16 +2862,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>102</v>
+        <v>198</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>103</v>
+        <v>178</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
@@ -2782,7 +2879,7 @@
         <v>7</v>
       </c>
       <c r="I56" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="12" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -2790,16 +2887,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>104</v>
+        <v>199</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>170</v>
+        <v>82</v>
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
@@ -2807,7 +2904,7 @@
         <v>7</v>
       </c>
       <c r="I57" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="12" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
@@ -2815,16 +2912,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="F58" s="16"/>
       <c r="G58" s="16"/>
@@ -2832,7 +2929,7 @@
         <v>7</v>
       </c>
       <c r="I58" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="12" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2840,16 +2937,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="C59" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>109</v>
+        <v>180</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>171</v>
+        <v>83</v>
       </c>
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
@@ -2857,7 +2954,7 @@
         <v>7</v>
       </c>
       <c r="I59" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="12" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2865,16 +2962,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>8</v>
+        <v>181</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>172</v>
+        <v>84</v>
       </c>
       <c r="F60" s="16"/>
       <c r="G60" s="16"/>
@@ -2882,7 +2979,7 @@
         <v>7</v>
       </c>
       <c r="I60" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="12" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -2890,16 +2987,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>112</v>
+        <v>182</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="F61" s="16"/>
       <c r="G61" s="16"/>
@@ -2907,7 +3004,7 @@
         <v>7</v>
       </c>
       <c r="I61" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="12" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
@@ -2915,16 +3012,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>114</v>
+        <v>183</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
       <c r="F62" s="16"/>
       <c r="G62" s="16"/>
@@ -2932,7 +3029,7 @@
         <v>7</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -2940,10 +3037,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
@@ -2952,6 +3049,13 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B35" r:id="rId1" xr:uid="{0B0644CE-3C4C-C54C-A78D-C149D076D413}"/>
+    <hyperlink ref="B50" r:id="rId2" xr:uid="{7CBCC04C-88E1-8441-B6A3-938A06076417}"/>
+    <hyperlink ref="B41" r:id="rId3" xr:uid="{F890F3E8-5639-704C-8358-B061B6626087}"/>
+    <hyperlink ref="B43" r:id="rId4" xr:uid="{D710FCB2-95DD-1142-8D75-E76FFD4AFAF4}"/>
+    <hyperlink ref="B45" r:id="rId5" xr:uid="{AC6B0EAB-8CD5-AD41-BB50-60B8FAF4128A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
last change for backsurvey behind gateway
</commit_message>
<xml_diff>
--- a/Back_Questionnaire.xlsx
+++ b/Back_Questionnaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanpro/Dropbox/Equal/git-perdev-dev/equal-survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AE0B7F-AE45-7847-A717-A43CF634328C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF21FC9B-CFC6-E444-BBB7-8B7519A97A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37300" yWindow="3020" windowWidth="29460" windowHeight="23340" xr2:uid="{C96B8C69-CC42-2D4D-A209-28F3A5CB5315}"/>
+    <workbookView xWindow="38640" yWindow="1900" windowWidth="29460" windowHeight="23340" xr2:uid="{C96B8C69-CC42-2D4D-A209-28F3A5CB5315}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,10 +189,6 @@
 </t>
   </si>
   <si>
-    <t>SET(@booster_vaccination)
-IF(@gender==female) THEN (GOTO: 3) ELSE (GOTO: 6)</t>
-  </si>
-  <si>
     <t>SET(@vomiting_reflux)</t>
   </si>
   <si>
@@ -387,11 +383,6 @@
   <si>
     <t>yes: 네, 매달 예방하고 있어요.
 no: 아니오, 매달 예방하지 않아요.</t>
-  </si>
-  <si>
-    <t>yes: 네, 추가 접종하고 있어요.
-conditional: 항제가검사를 통해 필요한 추가 접종만 진행하고 있어요.
-no: 아니오, 추가 접종하지 않아요.</t>
   </si>
   <si>
     <t>yes: 현재 임신 중.
@@ -949,7 +940,16 @@
 IF(@pet_type==dog) THEN (GOTO: 34) ELSE (GOTO: 45)</t>
   </si>
   <si>
-    <t>REDIRECT: home</t>
+    <t>REDIRECT: /get-report/{user_id}/{@petname}</t>
+  </si>
+  <si>
+    <t>SET(@booster_vaccination)
+IF(@gender==F) THEN (GOTO: 3) ELSE (GOTO: 6)</t>
+  </si>
+  <si>
+    <t>yes: 네, 추가 접종하고 있어요.
+conditional: 항체가 검사를 통해 필요한 추가 접종만 진행하고 있어요.
+no: 아니오, 추가 접종하지 않아요.</t>
   </si>
 </sst>
 </file>
@@ -1457,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5C60D7-EAD3-EB46-856C-21C3EE23727A}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,7 +1511,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>40</v>
@@ -1536,10 +1536,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>100</v>
+        <v>207</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -1555,16 +1555,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1572,7 +1572,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1586,10 +1586,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1597,7 +1597,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1611,7 +1611,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>36</v>
@@ -1622,7 +1622,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -1636,10 +1636,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -1655,13 +1655,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>37</v>
@@ -1672,7 +1672,7 @@
         <v>3</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="133" customHeight="1" x14ac:dyDescent="0.2">
@@ -1680,13 +1680,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>38</v>
@@ -1707,13 +1707,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>39</v>
@@ -1740,13 +1740,13 @@
         <v>10</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="11">
@@ -1767,20 +1767,20 @@
         <v>7</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18">
         <v>3</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.2">
@@ -1794,10 +1794,10 @@
         <v>10</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -1813,16 +1813,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -1844,10 +1844,10 @@
         <v>10</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -1863,16 +1863,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1880,7 +1880,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1888,16 +1888,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -1919,10 +1919,10 @@
         <v>10</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -1938,16 +1938,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1955,7 +1955,7 @@
         <v>3</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -1969,10 +1969,10 @@
         <v>10</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -1980,7 +1980,7 @@
         <v>3</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -1988,16 +1988,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -2005,7 +2005,7 @@
         <v>3</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -2019,10 +2019,10 @@
         <v>10</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2030,7 +2030,7 @@
         <v>4</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2044,10 +2044,10 @@
         <v>7</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -2055,7 +2055,7 @@
         <v>4</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2069,10 +2069,10 @@
         <v>10</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -2080,7 +2080,7 @@
         <v>4</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2094,10 +2094,10 @@
         <v>7</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -2105,7 +2105,7 @@
         <v>4</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2113,16 +2113,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -2138,16 +2138,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
@@ -2163,16 +2163,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
@@ -2188,16 +2188,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -2213,16 +2213,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -2238,16 +2238,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
@@ -2269,10 +2269,10 @@
         <v>7</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
@@ -2280,7 +2280,7 @@
         <v>4</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.2">
@@ -2294,10 +2294,10 @@
         <v>10</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
@@ -2305,7 +2305,7 @@
         <v>4</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.2">
@@ -2313,16 +2313,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -2344,10 +2344,10 @@
         <v>10</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -2363,7 +2363,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>10</v>
@@ -2372,7 +2372,7 @@
         <v>26</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2388,16 +2388,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2413,16 +2413,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2447,7 +2447,7 @@
         <v>28</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2463,16 +2463,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -2488,16 +2488,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
@@ -2513,16 +2513,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2538,16 +2538,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2563,16 +2563,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2588,16 +2588,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -2613,16 +2613,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
@@ -2638,7 +2638,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>10</v>
@@ -2647,7 +2647,7 @@
         <v>30</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
@@ -2663,16 +2663,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
@@ -2694,10 +2694,10 @@
         <v>10</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
@@ -2713,16 +2713,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
@@ -2738,16 +2738,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
@@ -2763,16 +2763,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
@@ -2788,19 +2788,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="18">
@@ -2815,16 +2815,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F54" s="16"/>
       <c r="G54" s="16"/>
@@ -2840,16 +2840,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F55" s="16"/>
       <c r="G55" s="16"/>
@@ -2865,16 +2865,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
@@ -2890,16 +2890,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
@@ -2921,10 +2921,10 @@
         <v>10</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F58" s="16"/>
       <c r="G58" s="16"/>
@@ -2940,16 +2940,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C59" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
@@ -2965,16 +2965,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F60" s="16"/>
       <c r="G60" s="16"/>
@@ -2996,10 +2996,10 @@
         <v>10</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F61" s="16"/>
       <c r="G61" s="16"/>
@@ -3015,16 +3015,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C62" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F62" s="16"/>
       <c r="G62" s="16"/>
@@ -3046,7 +3046,7 @@
         <v>35</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>

</xml_diff>

<commit_message>
change for 이/가 은/는 ... and remove in history
</commit_message>
<xml_diff>
--- a/Back_Questionnaire.xlsx
+++ b/Back_Questionnaire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanpro/Dropbox/Equal/git-perdev-dev/equal-survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF21FC9B-CFC6-E444-BBB7-8B7519A97A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3760D67-880C-F349-AD84-9FA9611248B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38640" yWindow="1900" windowWidth="29460" windowHeight="23340" xr2:uid="{C96B8C69-CC42-2D4D-A209-28F3A5CB5315}"/>
+    <workbookView xWindow="240" yWindow="1780" windowWidth="40640" windowHeight="23340" xr2:uid="{C96B8C69-CC42-2D4D-A209-28F3A5CB5315}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,29 +116,10 @@
     <t>dog</t>
   </si>
   <si>
-    <t>none: 아니요, 없었어요.
-reduced_reaction: 네, 쓰다듬거나 만졌을 때 예전보다 반응의 정도가 덜 해요.
-recognition_loss: 네, 갑자기 저를 못 알아보거나 무시해요.
-aggression: 네, 어딜 만지든 짖거나 물려고 해요.
-specific_aggression: 네, 특정 부위를 만지려고 하면 짖거나 물려고 해요.</t>
-  </si>
-  <si>
     <t>산책할 때 {@petname}의 상태는 어떤가요?</t>
   </si>
   <si>
-    <t>high: 계속 활발하게 걸어요.
-low: 처음부터 힘들어해요.
-low_after_short_walk: 10분 정도 걸으면 힘들어해요.
-low_after_medium_walk: 30분 정도 걸으면 힘들어해요.
-low_after_long_walk: 1시간 정도 걸으면 힘들어해요.</t>
-  </si>
-  <si>
     <t>cat</t>
-  </si>
-  <si>
-    <t>friendly: 친근하게 반겨줘요.
-indifferent: 저에게 딱히 관심을 보이지 않고 하던 일을 해요.
-fearful: 도망가거나 숨어있어요.</t>
   </si>
   <si>
     <t>주로 생활하는 공간은 어디인가요?</t>
@@ -177,9 +158,6 @@
   </si>
   <si>
     <t>Design</t>
-  </si>
-  <si>
-    <t>두 가지 이상의 사료를 먹는다면, 가장 많은 비중을 차지하는 사료를 기준으로 선택해주세요.</t>
   </si>
   <si>
     <t>주로 어떤 간식을 먹나요?</t>
@@ -381,46 +359,11 @@
 IF(@observation==difficult) THEN (GOTO:62) ELSE (GOTO:53)</t>
   </si>
   <si>
-    <t>yes: 네, 매달 예방하고 있어요.
-no: 아니오, 매달 예방하지 않아요.</t>
-  </si>
-  <si>
-    <t>yes: 현재 임신 중.
-no: 해당 없음.</t>
-  </si>
-  <si>
-    <t>yes: 출산한 적 있음.
-no: 해당 없음</t>
-  </si>
-  <si>
-    <t>yes: 현재 수유 중.
-no: 해당 없음</t>
-  </si>
-  <si>
-    <t>decreased_significantly: 눈에 띄게 줄었어요.
-decreased_slightly: 조금 줄었어요.
-no_change: 비슷해요.
-increased_slightly: 조금 늘었어요.
-increased_significantly: 눈에 띄게 늘었어요.</t>
-  </si>
-  <si>
     <t>고양이 헤르페스 바이러스 감염 증상(재채기, 콧물, 결막염 등)이 현재 있나요?</t>
-  </si>
-  <si>
-    <t>positive: 네, 증상이 있어요.
-negative: 아니오, 증상이 없어요.
-carrier: 증상은 없지만, 보균자예요.</t>
   </si>
   <si>
     <t xml:space="preserve">주로 어떤 사료를 먹이나요?
 </t>
-  </si>
-  <si>
-    <t>animal_protein: 동물성 단백질 일반 사료 (곤충 단백질 포함)
-plant_protein: 식물성 단백질 일반 사료&lt;br&gt;(두부, 콩 단백질 등이 포함돼요.)
-prescription_diet: 수의사 처방 사료&lt;br&gt;(Royal Canin, Hill's, Purina, Velixer 등에서 생산한 처방식을 이야기해요.)
-cooked_meat: 화식류 제품&lt;br&gt;(기성 제품 또는 집에서 직접 굽는 등 조리한 고기 등이 포함돼요.)
-raw_diet: 생식 및 동결건조 사료&lt;br&gt;(조리 안 된 어류, 육류 등이 포함돼요.)</t>
   </si>
   <si>
     <t>무슨 목적의 처방 사료인가요?</t>
@@ -448,28 +391,7 @@
     </r>
   </si>
   <si>
-    <t>recommended_or_less: 권장량만큼 주거나, 적게 줘요.
-more_than_recommended: 권장량보다 많이 줘요.</t>
-  </si>
-  <si>
-    <t>fast: 주자마자 순식간에 잘 씹지 않고 삼켜요.
-moderate: 적당한 속도로 잘 씹어서 먹어요.
-slow: 느리게 먹거나, 큰 관심이 없어 보여요.</t>
-  </si>
-  <si>
     <t>최근 구토 또는 역류 증상이 있었나요?</t>
-  </si>
-  <si>
-    <t>absent: 아니요.
-intermittent: 네, 종종 있어요.
-increased_recently: 최근 들어 심해졌어요.</t>
-  </si>
-  <si>
-    <t>dry_hard: 건조하고 딱딱해요.
-dry_soft: 건조한 편이지만, 말랑해요.
-moist_soft: 습기가 있으면서 적당히 말랑해요. 항문 주변에 살짝 묻어날 때도 있어요.
-loose: 변이 물러요. 항문 주변에 많이 묻어나요.
-diarrhea : 설사를 해요.</t>
   </si>
   <si>
     <r>
@@ -495,11 +417,6 @@
     </r>
   </si>
   <si>
-    <t>no: 아니오, 변비는 없어요.
-recent: 네, 최근에 변비가 생겼어요.
-chronic: 예전부터 변비가 있었어요.</t>
-  </si>
-  <si>
     <t>최근 음수량에 변화가 있었나요?</t>
   </si>
   <si>
@@ -539,137 +456,13 @@
     <t>미끄럼 방지 제품을 사용하시나요?</t>
   </si>
   <si>
-    <t>지금부터는 관찰이 필요해요. 답변을 한다면, 더 정교한 결과를 받을 수 있어요.</t>
-  </si>
-  <si>
-    <t>ready: 좋아요, 이어서 할게요!
-difficult: 지금은 어려워요.</t>
-  </si>
-  <si>
     <t>귓구멍의 증상이 양 쪽에서 나타나나요?</t>
   </si>
   <si>
     <t>탈모 증상이 있나요?</t>
   </si>
   <si>
-    <t>decreased: 음수량이 줄었어요.
-stable: 음수량이 그대로예요.
-increase: 음수량이 늘었어요.</t>
-  </si>
-  <si>
-    <t>decreased: 소변량이 줄었어요.
-stable: 소변량이 그대로예요.
-increased: 소변량이 늘었어요.</t>
-  </si>
-  <si>
-    <t>decreased: 소변 횟수가 줄었어요.
-stable: 소변 횟수가 그대로예요.
-increased: 소변 횟수가 늘었어요.</t>
-  </si>
-  <si>
-    <t>normal: 아니오, 그대로예요.
-strong: 네, 소변 냄새가 심해졌어요.</t>
-  </si>
-  <si>
-    <t>decreased: 화장실 방문을 평소보다 덜 해요.
-stable: 평소와 비슷하게 화장실을 방문해요.
-increased: 화장실 방문을 평소보다 자주 해요.</t>
-  </si>
-  <si>
-    <t>no_bathing: 목욕을 안 해요.
-less_than_monthly: 월에 1회 목욕해요.
-biweekly: 2주에 1회 목욕해요.
-weekly: 1주에 1회 목욕해요.
-twice_weekly: 1주에 2회 목욕해요.
-more_than_twice_weekly: 1주에 3회 이상 목욕해요.</t>
-  </si>
-  <si>
-    <t>regular:네, 주기적으로 미용해요.
-not_regular: 아니오, 주기적으로 미용하지 않아요.</t>
-  </si>
-  <si>
-    <t>home: 집에서 직접 미용해요.
-shop_or_vet: 샵이나 병원에서 미용해요.</t>
-  </si>
-  <si>
-    <t>yes: 네, 마취해요.
-no: 아니오, 마취하지 않아요.</t>
-  </si>
-  <si>
-    <t>yes: 네, 2회 이상 발생했어요.
-no: 아니오, 2회 이상 발생하지 않았어요.</t>
-  </si>
-  <si>
-    <t>not_dry: 건조해서 가습기를 틀어놔요.
-humid: 건조하지 않아요.
-dry_with_humidifier: 습한 편이에요.
-dry_without_care: 건조한 편이지만 특별히 신경 쓰고 있지 않아요.</t>
-  </si>
-  <si>
-    <t>never: 아니요, 그렇지 않아요.
-1-2_times_weekly: 주에 1~2회 드물게 보여요.
-3-5_times_weekly: 주에 3~5회 종종 보여요.
-daily: 거의 매일 보여요.</t>
-  </si>
-  <si>
-    <t>absent: 염증이나 구취가 없어요.
-present: 염증은 있지만, 구취가 심해지지 않았어요.
-worsened: 염증이 있고, 구취가 전보다 심해졌어요.
-unconfirmed: 입 안을 안 보여줘서 확인이 어려워요.</t>
-  </si>
-  <si>
     <t>가장 최근 스케일링은 언제인가요?</t>
-  </si>
-  <si>
-    <t>last_6_months: 6개월 내에 스케일링을 받았어요.
-6_months_to_1_year: 6개월~1년 사이에 스케일링을 받았어요.
-over_1_year_or_never: 받은지 1년이 넘었거나, 받은 적이 없어요.</t>
-  </si>
-  <si>
-    <t>everyday:매일 칫솔질을 해요.
-3_times_weekly: 주에 3회 이상 칫솔질을 해요.
-only_toothpaste: 치약을 잇몸과 치아에 발라주거나, 마시는 물에 치석 방지 제품을 섞어주기만 해요.
-never: 잘 해주지 않고 있어요.</t>
-  </si>
-  <si>
-    <t>yes: 네, 그런 경우가 있어요.
-no: 아니오, 그렇지 않아요.</t>
-  </si>
-  <si>
-    <t>never: 아니오, 그렇지 않아요.
-1-2_times_weekly: 주에 1~2회 비정상적인 숨소리를 내요.
-3-5_times_weekly: 주에 3~5회 비정상적인 숨소리를 내요.
-daily: 매일 비정상적인 숨소리를 내요.</t>
-  </si>
-  <si>
-    <t>none: 아니오, 그렇지 않아요.
-occasional: 운동을 격하게 했거나, 많이 흥분했을 때에만 캑캑거려요.
-frequent: 특별한 일이 없어도 캑캑거리는 모습이 하루에 한두 번 가끔 보여요.
-very_frequent: 특별한 일이 없어도 캑캑거리는 모습이 하루에 3~5회 이상 자주 보여요.</t>
-  </si>
-  <si>
-    <t>excitable: 항상 흥분한 상태예요.
-calm_excitable: 때로는 격하지만, 평소에는 차분한 편이에요.
-peaceful_expressive: 꼬리를 살랑이거나 만져달라고 오는 등 평온한 방식으로 기분과 상태를 표현해요.
-indifferent: 주변 환경 변화에 예민한 편은 아니에요. 성격이 무던해요.
-anxious_sensitive: 겁이 많고, 반려인과 멀어지거나 환경이 변화하면 많이 불안해하고 예민한 편이에요.</t>
-  </si>
-  <si>
-    <t>immediate_barking: 나가자마자 짖기 시작해요.
-occasional_barking: 나간 직후는 아니지만, 종종 짖기도 해요.
-indifferent: 크게 신경쓰지 않아 해요.</t>
-  </si>
-  <si>
-    <t>none: 산책을 거의 하지 않고, 활동량이 적어요.
-short: 하루에 30분 이내로 산책해요.
-medium: 하루에 30분 이상 60분 이내로 산책해요.
-long: 하루에 1시간 이상씩 산책해요.
-indoor: 산책을 자주 안 가지만, 실내 활동량이 많아요.</t>
-  </si>
-  <si>
-    <t>no_symptoms: 아니요, 그렇지 않아요.
-unstable_after_short_walk: 조금만 걸어도 다리를 떨거나 절뚝이는 등 불안정해 보여요.
-unstable_after_long_walk: 오래 걸으면 다리를 떨거나 절뚝이는 등 불안정해 보여요.</t>
   </si>
   <si>
     <t>slippery: 대리석 같이 미끄러운 바닥
@@ -677,120 +470,7 @@
 non_slippery: 장판 같이 미끄러짐이 거의 없는 바닥</t>
   </si>
   <si>
-    <t>low: 좌식 생활을 하는 중이거나, 소파나 침대가 낮은 편이에요.
-high: 소파나 침대가 높은 편이에요.
-high_stepped: 소파나 침대가 높은 편이지만, 계단식 구조물이 함께 있어요.</t>
-  </si>
-  <si>
-    <t>runs_and_jumps: 달려와서 점프해요.
-requests_assistance: 올려달라고 애원해요.
-uses_stairs_or_objects: 계단이나 주변 사물을 이용해서 올라와요.
-avoids_climbing: 잘 올라오지 않아요.</t>
-  </si>
-  <si>
-    <t>infrequent_standing: 두 발로 거의 서지 않아요.
-prevent_standing: 서자마자 바로 안아주거나 지시하는 등 최대한 두 발로 서지 않게 해요.
-indifferent: 크게 신경쓰지 않아요.</t>
-  </si>
-  <si>
-    <t>normal: 거의 숨지 않아요.
-occasional: 가끔 숨어요.
-increased: 최근에 더 숨는 편이에요.
-constant: 늘 숨고, 손길을 피해요.</t>
-  </si>
-  <si>
-    <t>sociable: 친근하게 다가가요.
-avoidant: 도망가거나 숨어요.
-defensive_aggressive: 방어 태세를 취하거나, 공격성을 보여요.
-indifferent: 사람에게 큰 관심이 없어요.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">indoor: 실내에서만 생활하고 외출하지 않아요.
-outdoor: 자유롭게 외출할 수 있어요.&lt;br&gt;(마당냥이나 길냥이를 포함해요.)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>other: 직접 작성하기</t>
-    </r>
-  </si>
-  <si>
-    <t>high_different_visitors: 네, 다른 외부인이 자주 방문해요.
-high_repeated_visitors: 네, 여러 번 왔던 외부인이 자주 방문해요.
-low_recent_increase: 아니오, 최근에만 외부인의 방문이 잦았어요.
-low_family_only: 아니오, 가족들만 출입해요.</t>
-  </si>
-  <si>
-    <t>yes: 네, 높은 가구가 있어요.
-no: 아니오, 높은 가구가 없어요.</t>
-  </si>
-  <si>
-    <t>high: 아니오, 집사가 지칠 때까지 계속 놀아요.
-moderate: 보통 지치지 않고 잘 놀지만, 주에 1~2회는 먼저 놀이를 멈추거나 쉬고 싶어 해요.
-low: 주에 3~4회 먼저 놀이를 멈추거나 쉬고 싶어 해요.
-very_low: 대부분 먼저 놀이를 멈추거나 쉬고 싶어 해요.</t>
-  </si>
-  <si>
-    <t>moist: 네, 잇몸이 촉촉해요.
-dry: 아니오, 잇몸이 건조해요.
-unknown: 보여주지 않아 확인하기 어려워요.</t>
-  </si>
-  <si>
-    <t>normal: 아니오, 충혈되지 않았어요.
-mild_congestion: 네, 약간 충혈되어 있어요.
-severe_congestion: 네, 심하게 충혈되어 있어요.</t>
-  </si>
-  <si>
-    <t>cloudy: 네, 그런 부분이 있어요.
-clear: 아니오, 그렇지 않아요.</t>
-  </si>
-  <si>
-    <t>moist: 네, 코가 촉촉해요.
-moist_with_discharge: 네, 그런데 하얗거나 노란 콧물을 동반하고 있어요.
-dry: 아니오, 코가 건조해요.</t>
-  </si>
-  <si>
-    <t>normal: 정상처럼 보여요.
-light_yellow_earwax: 연노란색 귀지가 많아요.
-brown_earwax: 갈색 귀지가 많아요.
-narrowed_earhole: 귀지 여부와 상관 없이 귓구멍이 좁아진 것처럼 보여요.
-reddened: 붉게 충혈됐어요.
-unconfirmed: 보여주지 않아 확인하기 어려워요.</t>
-  </si>
-  <si>
-    <t>bilateral: 네, 양 쪽 모두에서 나타나요.
-unilateral: 아니오, 한 쪽에서만 나타나요.</t>
-  </si>
-  <si>
-    <t>yes: 네, 있어요.
-no: 아니오, 없어요.</t>
-  </si>
-  <si>
-    <t>clumped: 네, 하지만 뭉치고 영겨 있어요.
-shiny: 네, 적당히 윤기가 있고 매끄러워요.
-dull: 아니오, 푸석해요.</t>
-  </si>
-  <si>
-    <t>no_symptoms: 아니오, 탈모 증상은 없어요.
-localized: 네, 한 곳에서만 털이 빠져요.
-symmetrical: 네, 대칭적으로 여러 곳에서 빠져요.
-asymmetrical: 네, 비대칭적으로 여러 곳에서 빠져요.
-generalized: 네, 전신에서 털이 빠져요.</t>
-  </si>
-  <si>
-    <t>두 가지 이상의 간식을 먹는다면, 가장 많은 비중을 차지하는 간식을 기준으로 선택해주세요.</t>
-  </si>
-  <si>
     <t>*권장 하루 간식 복용량: 하루 사료량의 10% 이하</t>
-  </si>
-  <si>
-    <t>아이의 눈, 코, 귓구멍, 털의 상태와 상처 여부를 안다면 이어서 답변할 수 있어요. (총 8~9문항)</t>
   </si>
   <si>
     <t>현재 {@petname}이 임신 중인가요?</t>
@@ -841,122 +521,382 @@
 none_used: 아무 것도 사용하지 않음</t>
   </si>
   <si>
+    <t>{@petname}이 주로 생활하는 환경에 외부인의 출입이 잦은 편인가요?</t>
+  </si>
+  <si>
+    <t>{@petname}이 주로 생활하는 실내 공간의 바닥은 어떤가요?</t>
+  </si>
+  <si>
+    <t>{@petname}이 주로 생활하는 실내 공간의 가구 높이는 어떤가요?</t>
+  </si>
+  <si>
+    <t>{@petname}이 두 발로 서려고 할 때, 반려인 님은 어떻게 반응하시나요?</t>
+  </si>
+  <si>
+    <t>SET(@weight_change)
+IF (@pet_type==cat) THEN (GOTO: 7) ELSE (GOTO:8)</t>
+  </si>
+  <si>
+    <t>SET(@fecal_condition)
+IF(@pet_type==cat) THEN (GOTO: 15) ELSE (GOTO:16)</t>
+  </si>
+  <si>
+    <t>SET(@urine_volume)
+IF(@pet_type==dog) THEN (GOTO: 18) ELSE (GOTO:19)</t>
+  </si>
+  <si>
+    <t>SET(@urine_odor)
+IF(@pet_type==cat) THEN (GOTO: 20) ELSE (GOTO:21)</t>
+  </si>
+  <si>
+    <t>SET(@toothbrushing)
+IF(@pet_type==cat) THEN (GOTO: 31) ELSE (GOTO: 32)</t>
+  </si>
+  <si>
+    <t>SET(@coughing_frequency)
+IF(@pet_type==dog) THEN (GOTO: 34) ELSE (GOTO: 45)</t>
+  </si>
+  <si>
+    <t>REDIRECT: /get-report/{user_id}/{@petname}</t>
+  </si>
+  <si>
+    <t>SET(@booster_vaccination)
+IF(@gender==F) THEN (GOTO: 3) ELSE (GOTO: 6)</t>
+  </si>
+  <si>
     <t>SET(@ear_condition)
-IF(@ear_condition==normal) THEN (GOTO:59)
-ELIF(@ear_condition==unconfirmed) THEN (GOTO:59)
-GOTO:58</t>
-  </si>
-  <si>
-    <t>{@petname}이 주로 생활하는 환경에 외부인의 출입이 잦은 편인가요?</t>
-  </si>
-  <si>
-    <t>{@petname}이 주로 생활하는 실내 공간의 바닥은 어떤가요?</t>
-  </si>
-  <si>
-    <t>{@petname}이 주로 생활하는 실내 공간의 가구 높이는 어떤가요?</t>
-  </si>
-  <si>
-    <t>{@petname}이 두 발로 서려고 할 때, 반려인 님은 어떻게 반응하시나요?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">none: 간식을 먹지 않아요.
-wet_snacks: 습식 간식류&lt;br&gt;(츄르, 양갱, 퓨레, 무스, 동물용 통조림 등이 있어요.)
-dry_snacks: 건식 간식류&lt;br&gt;(동결건조, 쿠키, 육포, 저키 등이 있어요.)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>functional_snacks: 기능성 간식류&lt;br&gt;(오메가3, 유산균 등 특정한 건강보조성분이 포함된 간식류를 말해요.)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>IF(@pet_type==dog) THEN (dog_dental_chew: 개껌류)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+IF(@ear_condition==normal) THEN (GOTO:59) ELIF(@ear_condition==unconfirmed) THEN (GOTO:59) ELSE (GOTO:58)</t>
+  </si>
+  <si>
+    <t>yes: 현재 임신 중
+no: 해당 없음</t>
+  </si>
+  <si>
+    <t>yes: 출산한 적 있음
+no: 해당 없음</t>
+  </si>
+  <si>
+    <t>yes: 현재 수유 중
+no: 해당 없음</t>
+  </si>
+  <si>
+    <t>decreased_significantly: 눈에 띄게 줄었어요
+decreased_slightly: 조금 줄었어요
+no_change: 비슷해요
+increased_slightly: 조금 늘었어요
+increased_significantly: 눈에 띄게 늘었어요</t>
+  </si>
+  <si>
+    <t>yes: 네, 매달 예방하고 있어요
+no: 아니오, 매달 예방하지 않아요</t>
+  </si>
+  <si>
+    <t>yes: 네, 추가 접종하고 있어요
+conditional: 항체가 검사를 통해 필요한 추가 접종만 진행하고 있어요
+no: 아니오, 추가 접종하지 않아요</t>
+  </si>
+  <si>
+    <t>positive: 네, 증상이 있어요
+negative: 아니오, 증상이 없어요
+carrier: 증상은 없지만, 보균자예요</t>
+  </si>
+  <si>
+    <t>recommended_or_less: 권장량만큼 주거나, 적게 줘요
+more_than_recommended: 권장량보다 많이 줘요</t>
+  </si>
+  <si>
+    <t>fast: 주자마자 순식간에 잘 씹지 않고 삼켜요
+moderate: 적당한 속도로 잘 씹어서 먹어요
+slow: 느리게 먹거나, 큰 관심이 없어 보여요</t>
+  </si>
+  <si>
+    <t>absent: 아니요
+intermittent: 네, 종종 있어요
+increased_recently: 최근 들어 심해졌어요</t>
+  </si>
+  <si>
+    <t>animal_protein: 동물성 단백질 일반 사료 (곤충 단백질 포함)
+plant_protein: 식물성 단백질 일반 사료&lt;br&gt;(두부, 콩 단백질 등이 포함돼요)
+prescription_diet: 수의사 처방 사료&lt;br&gt;(Royal Canin, Hill's, Purina, Velixer 등에서 생산한 처방식을 이야기해요)
+cooked_meat: 화식류 제품&lt;br&gt;(기성 제품 또는 집에서 직접 굽는 등 조리한 고기 등이 포함돼요)
+raw_diet: 생식 및 동결건조 사료&lt;br&gt;(조리 안 된 어류, 육류 등이 포함돼요)</t>
+  </si>
+  <si>
+    <t>두 가지 이상의 사료를 먹는다면, 가장 많은 비중을 차지하는 사료를 기준으로 선택해주세요</t>
+  </si>
+  <si>
+    <t>none: 간식을 먹지 않아요
+wet_snacks: 습식 간식류&lt;br&gt;(츄르, 양갱, 퓨레, 무스, 동물용 통조림 등이 있어요)
+dry_snacks: 건식 간식류&lt;br&gt;(동결건조, 쿠키, 육포, 저키 등이 있어요)
+functional_snacks: 기능성 간식류&lt;br&gt;(오메가3, 유산균 등 특정한 건강보조성분이 포함된 간식류를 말해요)
+IF(@pet_type==dog) THEN (dog_dental_chew: 개껌류)
 natural_fruit_vegetable: 천연 재료 간식류 중 과일, 야채 위주
 natural_meat: 천연 재료 간식류 중 육류 위주
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>other: 직접 작성하기</t>
-    </r>
-  </si>
-  <si>
-    <t>SET(@weight_change)
-IF (@pet_type==cat) THEN (GOTO: 7) ELSE (GOTO:8)</t>
-  </si>
-  <si>
-    <t>SET(@fecal_condition)
-IF(@pet_type==cat) THEN (GOTO: 15) ELSE (GOTO:16)</t>
-  </si>
-  <si>
-    <t>SET(@urine_volume)
-IF(@pet_type==dog) THEN (GOTO: 18) ELSE (GOTO:19)</t>
-  </si>
-  <si>
-    <t>SET(@urine_odor)
-IF(@pet_type==cat) THEN (GOTO: 20) ELSE (GOTO:21)</t>
-  </si>
-  <si>
-    <t>SET(@toothbrushing)
-IF(@pet_type==cat) THEN (GOTO: 31) ELSE (GOTO: 32)</t>
-  </si>
-  <si>
-    <t>SET(@coughing_frequency)
-IF(@pet_type==dog) THEN (GOTO: 34) ELSE (GOTO: 45)</t>
-  </si>
-  <si>
-    <t>REDIRECT: /get-report/{user_id}/{@petname}</t>
-  </si>
-  <si>
-    <t>SET(@booster_vaccination)
-IF(@gender==F) THEN (GOTO: 3) ELSE (GOTO: 6)</t>
-  </si>
-  <si>
-    <t>yes: 네, 추가 접종하고 있어요.
-conditional: 항체가 검사를 통해 필요한 추가 접종만 진행하고 있어요.
-no: 아니오, 추가 접종하지 않아요.</t>
+other: 직접 작성하기</t>
+  </si>
+  <si>
+    <t>두 가지 이상의 간식을 먹는다면, 가장 많은 비중을 차지하는 간식을 기준으로 선택해주세요</t>
+  </si>
+  <si>
+    <t>dry_hard: 건조하고 딱딱해요
+dry_soft: 건조한 편이지만, 말랑해요
+moist_soft: 습기가 있으면서 적당히 말랑해요 항문 주변에 살짝 묻어날 때도 있어요
+loose: 변이 물러요 항문 주변에 많이 묻어나요
+diarrhea : 설사를 해요</t>
+  </si>
+  <si>
+    <t>no: 아니오, 변비는 없어요
+recent: 네, 최근에 변비가 생겼어요
+chronic: 예전부터 변비가 있었어요</t>
+  </si>
+  <si>
+    <t>decreased: 음수량이 줄었어요
+stable: 음수량이 그대로예요
+increase: 음수량이 늘었어요</t>
+  </si>
+  <si>
+    <t>decreased: 소변량이 줄었어요
+stable: 소변량이 그대로예요
+increased: 소변량이 늘었어요</t>
+  </si>
+  <si>
+    <t>decreased: 소변 횟수가 줄었어요
+stable: 소변 횟수가 그대로예요
+increased: 소변 횟수가 늘었어요</t>
+  </si>
+  <si>
+    <t>normal: 아니오, 그대로예요
+strong: 네, 소변 냄새가 심해졌어요</t>
+  </si>
+  <si>
+    <t>decreased: 화장실 방문을 평소보다 덜 해요
+stable: 평소와 비슷하게 화장실을 방문해요
+increased: 화장실 방문을 평소보다 자주 해요</t>
+  </si>
+  <si>
+    <t>no_bathing: 목욕을 안 해요
+less_than_monthly: 월에 1회 목욕해요
+biweekly: 2주에 1회 목욕해요
+weekly: 1주에 1회 목욕해요
+twice_weekly: 1주에 2회 목욕해요
+more_than_twice_weekly: 1주에 3회 이상 목욕해요</t>
+  </si>
+  <si>
+    <t>regular:네, 주기적으로 미용해요
+not_regular: 아니오, 주기적으로 미용하지 않아요</t>
+  </si>
+  <si>
+    <t>home: 집에서 직접 미용해요
+shop_or_vet: 샵이나 병원에서 미용해요</t>
+  </si>
+  <si>
+    <t>yes: 네, 마취해요
+no: 아니오, 마취하지 않아요</t>
+  </si>
+  <si>
+    <t>yes: 네, 2회 이상 발생했어요
+no: 아니오, 2회 이상 발생하지 않았어요</t>
+  </si>
+  <si>
+    <t>not_dry: 건조해서 가습기를 틀어놔요
+humid: 건조하지 않아요
+dry_with_humidifier: 습한 편이에요
+dry_without_care: 건조한 편이지만 특별히 신경 쓰고 있지 않아요</t>
+  </si>
+  <si>
+    <t>never: 아니요, 그렇지 않아요
+1-2_times_weekly: 주에 1~2회 드물게 보여요
+3-5_times_weekly: 주에 3~5회 종종 보여요
+daily: 거의 매일 보여요</t>
+  </si>
+  <si>
+    <t>absent: 염증이나 구취가 없어요
+present: 염증은 있지만, 구취가 심해지지 않았어요
+worsened: 염증이 있고, 구취가 전보다 심해졌어요
+unconfirmed: 입 안을 안 보여줘서 확인이 어려워요</t>
+  </si>
+  <si>
+    <t>last_6_months: 6개월 내에 스케일링을 받았어요
+6_months_to_1_year: 6개월~1년 사이에 스케일링을 받았어요
+over_1_year_or_never: 받은지 1년이 넘었거나, 받은 적이 없어요</t>
+  </si>
+  <si>
+    <t>everyday:매일 칫솔질을 해요
+3_times_weekly: 주에 3회 이상 칫솔질을 해요
+only_toothpaste: 치약을 잇몸과 치아에 발라주거나, 마시는 물에 치석 방지 제품을 섞어주기만 해요
+never: 잘 해주지 않고 있어요</t>
+  </si>
+  <si>
+    <t>yes: 네, 그런 경우가 있어요
+no: 아니오, 그렇지 않아요</t>
+  </si>
+  <si>
+    <t>never: 아니오, 그렇지 않아요
+1-2_times_weekly: 주에 1~2회 비정상적인 숨소리를 내요
+3-5_times_weekly: 주에 3~5회 비정상적인 숨소리를 내요
+daily: 매일 비정상적인 숨소리를 내요</t>
+  </si>
+  <si>
+    <t>none: 아니오, 그렇지 않아요
+occasional: 운동을 격하게 했거나, 많이 흥분했을 때에만 캑캑거려요
+frequent: 특별한 일이 없어도 캑캑거리는 모습이 하루에 한두 번 가끔 보여요
+very_frequent: 특별한 일이 없어도 캑캑거리는 모습이 하루에 3~5회 이상 자주 보여요</t>
+  </si>
+  <si>
+    <t>excitable: 항상 흥분한 상태예요
+calm_excitable: 때로는 격하지만, 평소에는 차분한 편이에요
+peaceful_expressive: 꼬리를 살랑이거나 만져달라고 오는 등 평온한 방식으로 기분과 상태를 표현해요
+indifferent: 주변 환경 변화에 예민한 편은 아니에요 성격이 무던해요
+anxious_sensitive: 겁이 많고, 반려인과 멀어지거나 환경이 변화하면 많이 불안해하고 예민한 편이에요</t>
+  </si>
+  <si>
+    <t>none: 아니요, 없었어요
+reduced_reaction: 네, 쓰다듬거나 만졌을 때 예전보다 반응의 정도가 덜 해요
+recognition_loss: 네, 갑자기 저를 못 알아보거나 무시해요
+aggression: 네, 어딜 만지든 짖거나 물려고 해요
+specific_aggression: 네, 특정 부위를 만지려고 하면 짖거나 물려고 해요</t>
+  </si>
+  <si>
+    <t>immediate_barking: 나가자마자 짖기 시작해요
+occasional_barking: 나간 직후는 아니지만, 종종 짖기도 해요
+indifferent: 크게 신경쓰지 않아 해요</t>
+  </si>
+  <si>
+    <t>none: 산책을 거의 하지 않고, 활동량이 적어요
+short: 하루에 30분 이내로 산책해요
+medium: 하루에 30분 이상 60분 이내로 산책해요
+long: 하루에 1시간 이상씩 산책해요
+indoor: 산책을 자주 안 가지만, 실내 활동량이 많아요</t>
+  </si>
+  <si>
+    <t>high: 계속 활발하게 걸어요
+low: 처음부터 힘들어해요
+low_after_short_walk: 10분 정도 걸으면 힘들어해요
+low_after_medium_walk: 30분 정도 걸으면 힘들어해요
+low_after_long_walk: 1시간 정도 걸으면 힘들어해요</t>
+  </si>
+  <si>
+    <t>no_symptoms: 아니요, 그렇지 않아요
+unstable_after_short_walk: 조금만 걸어도 다리를 떨거나 절뚝이는 등 불안정해 보여요
+unstable_after_long_walk: 오래 걸으면 다리를 떨거나 절뚝이는 등 불안정해 보여요</t>
+  </si>
+  <si>
+    <t>low: 좌식 생활을 하는 중이거나, 소파나 침대가 낮은 편이에요
+high: 소파나 침대가 높은 편이에요
+high_stepped: 소파나 침대가 높은 편이지만, 계단식 구조물이 함께 있어요</t>
+  </si>
+  <si>
+    <t>runs_and_jumps: 달려와서 점프해요
+requests_assistance: 올려달라고 애원해요
+uses_stairs_or_objects: 계단이나 주변 사물을 이용해서 올라와요
+avoids_climbing: 잘 올라오지 않아요</t>
+  </si>
+  <si>
+    <t>infrequent_standing: 두 발로 거의 서지 않아요
+prevent_standing: 서자마자 바로 안아주거나 지시하는 등 최대한 두 발로 서지 않게 해요
+indifferent: 크게 신경쓰지 않아요</t>
+  </si>
+  <si>
+    <t>normal: 거의 숨지 않아요
+occasional: 가끔 숨어요
+increased: 최근에 더 숨는 편이에요
+constant: 늘 숨고, 손길을 피해요</t>
+  </si>
+  <si>
+    <t>friendly: 친근하게 반겨줘요
+indifferent: 저에게 딱히 관심을 보이지 않고 하던 일을 해요
+fearful: 도망가거나 숨어있어요</t>
+  </si>
+  <si>
+    <t>sociable: 친근하게 다가가요
+avoidant: 도망가거나 숨어요
+defensive_aggressive: 방어 태세를 취하거나, 공격성을 보여요
+indifferent: 사람에게 큰 관심이 없어요</t>
+  </si>
+  <si>
+    <t>indoor: 실내에서만 생활하고 외출하지 않아요
+outdoor: 자유롭게 외출할 수 있어요&lt;br&gt;(마당냥이나 길냥이를 포함해요)
+other: 직접 작성하기</t>
+  </si>
+  <si>
+    <t>high_different_visitors: 네, 다른 외부인이 자주 방문해요
+high_repeated_visitors: 네, 여러 번 왔던 외부인이 자주 방문해요
+low_recent_increase: 아니오, 최근에만 외부인의 방문이 잦았어요
+low_family_only: 아니오, 가족들만 출입해요</t>
+  </si>
+  <si>
+    <t>yes: 네, 높은 가구가 있어요
+no: 아니오, 높은 가구가 없어요</t>
+  </si>
+  <si>
+    <t>high: 아니오, 집사가 지칠 때까지 계속 놀아요
+moderate: 보통 지치지 않고 잘 놀지만, 주에 1~2회는 먼저 놀이를 멈추거나 쉬고 싶어 해요
+low: 주에 3~4회 먼저 놀이를 멈추거나 쉬고 싶어 해요
+very_low: 대부분 먼저 놀이를 멈추거나 쉬고 싶어 해요</t>
+  </si>
+  <si>
+    <t>지금부터는 관찰이 필요해요 답변을 한다면, 더 정교한 결과를 받을 수 있어요</t>
+  </si>
+  <si>
+    <t>ready: 좋아요, 이어서 할게요!
+difficult: 지금은 어려워요</t>
+  </si>
+  <si>
+    <t>아이의 눈, 코, 귓구멍, 털의 상태와 상처 여부를 안다면 이어서 답변할 수 있어요 (총 8~9문항)</t>
+  </si>
+  <si>
+    <t>normal: 아니오, 충혈되지 않았어요
+mild_congestion: 네, 약간 충혈되어 있어요
+severe_congestion: 네, 심하게 충혈되어 있어요</t>
+  </si>
+  <si>
+    <t>cloudy: 네, 그런 부분이 있어요
+clear: 아니오, 그렇지 않아요</t>
+  </si>
+  <si>
+    <t>moist: 네, 코가 촉촉해요
+moist_with_discharge: 네, 그런데 하얗거나 노란 콧물을 동반하고 있어요
+dry: 아니오, 코가 건조해요</t>
+  </si>
+  <si>
+    <t>moist: 네, 잇몸이 촉촉해요
+dry: 아니오, 잇몸이 건조해요
+unknown: 보여주지 않아 확인하기 어려워요</t>
+  </si>
+  <si>
+    <t>normal: 정상처럼 보여요
+light_yellow_earwax: 연노란색 귀지가 많아요
+brown_earwax: 갈색 귀지가 많아요
+narrowed_earhole: 귀지 여부와 상관 없이 귓구멍이 좁아진 것처럼 보여요
+reddened: 붉게 충혈됐어요
+unconfirmed: 보여주지 않아 확인하기 어려워요</t>
+  </si>
+  <si>
+    <t>bilateral: 네, 양 쪽 모두에서 나타나요
+unilateral: 아니오, 한 쪽에서만 나타나요</t>
+  </si>
+  <si>
+    <t>yes: 네, 있어요
+no: 아니오, 없어요</t>
+  </si>
+  <si>
+    <t>clumped: 네, 하지만 뭉치고 영겨 있어요
+shiny: 네, 적당히 윤기가 있고 매끄러워요
+dull: 아니오, 푸석해요</t>
+  </si>
+  <si>
+    <t>no_symptoms: 아니오, 탈모 증상은 없어요
+localized: 네, 한 곳에서만 털이 빠져요
+symmetrical: 네, 대칭적으로 여러 곳에서 빠져요
+asymmetrical: 네, 비대칭적으로 여러 곳에서 빠져요
+generalized: 네, 전신에서 털이 빠져요</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -978,10 +918,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri (Body)"/>
     </font>
     <font>
       <b/>
@@ -1064,7 +1000,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1127,10 +1063,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1457,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5C60D7-EAD3-EB46-856C-21C3EE23727A}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1467,7 +1403,7 @@
     <col min="2" max="2" width="42.5" style="7" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
     <col min="4" max="4" width="84.33203125" customWidth="1"/>
-    <col min="5" max="5" width="56.83203125" customWidth="1"/>
+    <col min="5" max="5" width="46.83203125" customWidth="1"/>
     <col min="6" max="6" width="32.1640625" customWidth="1"/>
     <col min="7" max="7" width="3.5" customWidth="1"/>
     <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -1491,10 +1427,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -1511,10 +1447,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
@@ -1536,10 +1472,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>207</v>
+        <v>151</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -1550,21 +1486,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>178</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1572,10 +1508,10 @@
         <v>2</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1586,10 +1522,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1597,7 +1533,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1611,10 +1547,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1622,7 +1558,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -1636,10 +1572,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>199</v>
+        <v>137</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -1655,16 +1591,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -1672,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="133" customHeight="1" x14ac:dyDescent="0.2">
@@ -1680,19 +1616,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>43</v>
+        <v>157</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="18">
@@ -1707,19 +1643,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>43</v>
+        <v>157</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18">
@@ -1734,19 +1670,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="11">
@@ -1761,26 +1697,26 @@
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>176</v>
+        <v>117</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18">
         <v>3</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.2">
@@ -1794,10 +1730,10 @@
         <v>10</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -1813,16 +1749,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>112</v>
+        <v>155</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -1844,10 +1780,10 @@
         <v>10</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>200</v>
+        <v>138</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -1863,16 +1799,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>115</v>
+        <v>161</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1880,7 +1816,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1888,16 +1824,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -1919,10 +1855,10 @@
         <v>10</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>201</v>
+        <v>139</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -1938,16 +1874,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1955,7 +1891,7 @@
         <v>3</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -1969,10 +1905,10 @@
         <v>10</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>202</v>
+        <v>140</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -1980,7 +1916,7 @@
         <v>3</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -1988,16 +1924,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -2005,7 +1941,7 @@
         <v>3</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -2019,10 +1955,10 @@
         <v>10</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2030,7 +1966,7 @@
         <v>4</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2044,10 +1980,10 @@
         <v>7</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -2055,10 +1991,10 @@
         <v>4</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <v>23</v>
       </c>
@@ -2069,10 +2005,10 @@
         <v>10</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -2080,7 +2016,7 @@
         <v>4</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2094,10 +2030,10 @@
         <v>7</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -2105,7 +2041,7 @@
         <v>4</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2113,16 +2049,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -2138,16 +2074,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
@@ -2163,16 +2099,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>181</v>
+        <v>121</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
@@ -2188,16 +2124,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -2213,16 +2149,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -2238,16 +2174,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>203</v>
+        <v>141</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
@@ -2269,10 +2205,10 @@
         <v>7</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
@@ -2280,7 +2216,7 @@
         <v>4</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.2">
@@ -2294,10 +2230,10 @@
         <v>10</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
@@ -2305,7 +2241,7 @@
         <v>4</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.2">
@@ -2313,16 +2249,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>204</v>
+        <v>142</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -2344,10 +2280,10 @@
         <v>10</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -2363,16 +2299,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>26</v>
+        <v>181</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2388,16 +2324,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="E37" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2413,16 +2349,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2438,16 +2374,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>28</v>
+        <v>184</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2463,16 +2399,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -2488,16 +2424,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>195</v>
+        <v>134</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
@@ -2513,16 +2449,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>192</v>
+        <v>132</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2538,16 +2474,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>196</v>
+        <v>135</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2563,16 +2499,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>183</v>
+        <v>123</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2588,16 +2524,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -2613,16 +2549,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>184</v>
+        <v>124</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
@@ -2630,7 +2566,7 @@
         <v>6</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="15" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -2638,16 +2574,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>185</v>
+        <v>125</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>30</v>
+        <v>190</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
@@ -2655,7 +2591,7 @@
         <v>6</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="15" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -2663,16 +2599,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>186</v>
+        <v>126</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
@@ -2680,7 +2616,7 @@
         <v>6</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="21" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
@@ -2688,16 +2624,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C49" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
@@ -2705,7 +2641,7 @@
         <v>6</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="15" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
@@ -2713,16 +2649,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>194</v>
+        <v>133</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
@@ -2730,7 +2666,7 @@
         <v>6</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -2738,16 +2674,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
@@ -2755,7 +2691,7 @@
         <v>6</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="15" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
@@ -2763,16 +2699,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
@@ -2780,7 +2716,7 @@
         <v>6</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="12" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
@@ -2788,19 +2724,19 @@
         <v>52</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>129</v>
+        <v>196</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>130</v>
+        <v>197</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="18">
@@ -2815,16 +2751,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>187</v>
+        <v>127</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F54" s="16"/>
       <c r="G54" s="16"/>
@@ -2840,16 +2776,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="C55" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F55" s="16"/>
       <c r="G55" s="16"/>
@@ -2865,16 +2801,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>189</v>
+        <v>129</v>
       </c>
       <c r="C56" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>169</v>
+        <v>201</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
@@ -2890,16 +2826,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>166</v>
+        <v>202</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
@@ -2915,16 +2851,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>193</v>
+        <v>145</v>
       </c>
       <c r="F58" s="16"/>
       <c r="G58" s="16"/>
@@ -2940,16 +2876,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C59" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
@@ -2965,16 +2901,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>191</v>
+        <v>131</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F60" s="16"/>
       <c r="G60" s="16"/>
@@ -2990,16 +2926,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C61" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>173</v>
+        <v>206</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F61" s="16"/>
       <c r="G61" s="16"/>
@@ -3015,16 +2951,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="C62" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F62" s="16"/>
       <c r="G62" s="16"/>
@@ -3040,13 +2976,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>205</v>
+        <v>143</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>

</xml_diff>